<commit_message>
updated currently reading books
</commit_message>
<xml_diff>
--- a/thongnd_everything_list.xlsx
+++ b/thongnd_everything_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\ドキュメント\GitHub\My_Everything_Lists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2458018F-97FF-4693-BD4C-D748F3BF18A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82280527-1195-4DDD-A30F-91B94913B014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1_todolist" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1854" uniqueCount="1253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1863" uniqueCount="1264">
   <si>
     <t>ID</t>
   </si>
@@ -3015,9 +3015,6 @@
   </si>
   <si>
     <t>the 4 hour work week</t>
-  </si>
-  <si>
-    <t>Atomic Habits: An Easy &amp; Proven Way to Build Good Habits &amp; Break Bad Ones</t>
   </si>
   <si>
     <t>すずみ。Suzume</t>
@@ -4629,22 +4626,6 @@
   </si>
   <si>
     <t>LANGUAGE LEARNING BOOKS</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <r>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>024.March, reading</t>
-    </r>
     <phoneticPr fontId="5"/>
   </si>
   <si>
@@ -5405,6 +5386,58 @@
   </si>
   <si>
     <t>shougun.</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>STATUS</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Definitive Guide to ARM Cortex-M0</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Started 2024</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>2024.March, reading</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Atomic Habits: An Easy &amp; Proven Way to Build Good Habits &amp; Break Bad Ones</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>The One Thing</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Gary Keller</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Start Nation</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Dropped</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>From Zero to One</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Peter Thiel</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>reading. Dropped</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>NAME</t>
     <phoneticPr fontId="5"/>
   </si>
 </sst>
@@ -6011,7 +6044,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D1043"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -6025,27 +6058,27 @@
   <sheetData>
     <row r="1" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="50" t="s">
-        <v>1233</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="2" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="22" t="s">
-        <v>1230</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="49" t="s">
-        <v>1231</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="49" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6053,25 +6086,25 @@
     </row>
     <row r="8" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="44" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="30" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="24" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="49" t="s">
-        <v>1232</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6082,22 +6115,22 @@
     </row>
     <row r="14" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="49" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="15" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
-        <v>1234</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="16" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="10" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="18" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6111,17 +6144,17 @@
     </row>
     <row r="21" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="50" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="22" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="11" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="23" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="24" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -6129,18 +6162,18 @@
     </row>
     <row r="25" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="11" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="26" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="28" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="22" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="29" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6151,18 +6184,18 @@
     </row>
     <row r="31" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="32" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="34" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="35" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -6170,50 +6203,50 @@
     </row>
     <row r="36" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="37" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="38" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="39" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="6" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="40" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="6" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="41" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="42" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="6" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="43" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="44" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="6" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="45" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -6221,17 +6254,17 @@
     </row>
     <row r="46" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="8" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="47" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="48" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6242,12 +6275,12 @@
     </row>
     <row r="51" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="38" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -6262,7 +6295,7 @@
     </row>
     <row r="55" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6271,7 +6304,7 @@
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="44" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -6357,7 +6390,7 @@
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
@@ -6476,7 +6509,7 @@
     <row r="90" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="91" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" s="3" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="92" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -6491,14 +6524,14 @@
     </row>
     <row r="94" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="95" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="96" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="97" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B97" s="3" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="98" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -6526,69 +6559,69 @@
     </row>
     <row r="102" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B102" s="1" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="103" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B103" s="6" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="104" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B104" s="6" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="105" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B105" s="6" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="107" spans="2:3" ht="55.5" x14ac:dyDescent="0.25">
       <c r="B107" s="37" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="C107" s="51" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="108" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B108" s="6" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C108" s="5" t="s">
         <v>1171</v>
-      </c>
-      <c r="C108" s="5" t="s">
-        <v>1172</v>
       </c>
     </row>
     <row r="109" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B109" s="6" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="110" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B110" s="6" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>1189</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="111" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B111" s="6" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="112" spans="2:3" ht="64.5" x14ac:dyDescent="0.25">
       <c r="B112" s="24" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="C112" s="45" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="113" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B113" s="1" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="114" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7584,7 +7617,7 @@
         <v>53</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>54</v>
@@ -7694,7 +7727,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
       <c r="C11" s="4"/>
       <c r="F11" s="1" t="s">
@@ -7736,7 +7769,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>1217</v>
+        <v>1215</v>
       </c>
       <c r="C14" s="4"/>
       <c r="F14" s="1" t="s">
@@ -7748,7 +7781,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="C15" s="4"/>
       <c r="F15" s="1" t="s">
@@ -7775,7 +7808,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>1218</v>
+        <v>1216</v>
       </c>
       <c r="C17" s="4"/>
       <c r="F17" s="1" t="s">
@@ -7923,14 +7956,14 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="C29" s="4"/>
       <c r="F29" s="1" t="s">
         <v>54</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -7938,7 +7971,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="C30" s="4">
         <v>2008</v>
@@ -8081,7 +8114,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="19">
@@ -8099,7 +8132,7 @@
         <v>95</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="D42" s="19">
         <v>42499</v>
@@ -8158,7 +8191,7 @@
         <v>99</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>54</v>
@@ -8172,7 +8205,7 @@
         <v>100</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>54</v>
@@ -8186,7 +8219,7 @@
         <v>101</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="E48" s="17" t="s">
         <v>102</v>
@@ -8254,7 +8287,7 @@
         <v>109</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="D52" s="19">
         <v>42468</v>
@@ -8274,7 +8307,7 @@
         <v>111</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="D53" s="19">
         <v>42498</v>
@@ -8294,7 +8327,7 @@
         <v>113</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="D54" s="19">
         <v>42529</v>
@@ -8357,7 +8390,7 @@
         <v>119</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="D57" s="19">
         <v>42712</v>
@@ -8380,7 +8413,7 @@
         <v>122</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="D58" s="19">
         <v>42605</v>
@@ -8397,7 +8430,7 @@
         <v>123</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="D59" s="19">
         <v>42560</v>
@@ -8440,7 +8473,7 @@
         <v>128</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="D61" s="19">
         <v>42665</v>
@@ -8505,7 +8538,7 @@
         <v>134</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="D65" s="19">
         <v>42756</v>
@@ -8543,7 +8576,7 @@
         <v>138</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="D67" s="19">
         <v>42757</v>
@@ -8643,13 +8676,13 @@
         <v>147</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="D72" s="19">
         <v>42838</v>
       </c>
       <c r="E72" s="17" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>54</v>
@@ -8663,7 +8696,7 @@
         <v>148</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="D73" s="19">
         <v>42963</v>
@@ -8686,7 +8719,7 @@
         <v>151</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="D74" s="19">
         <v>42980</v>
@@ -8706,7 +8739,7 @@
         <v>153</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="D75" s="19">
         <v>43007</v>
@@ -8726,7 +8759,7 @@
         <v>155</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="D76" s="19">
         <v>43019</v>
@@ -8740,7 +8773,7 @@
     </row>
     <row r="77" spans="1:7" s="33" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="33" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="C77" s="46">
         <v>2009</v>
@@ -8748,7 +8781,7 @@
       <c r="D77" s="34"/>
       <c r="E77" s="47"/>
       <c r="G77" s="33" t="s">
-        <v>1191</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -8869,7 +8902,7 @@
         <v>54</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -8881,7 +8914,7 @@
         <v>166</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="D84" s="19">
         <v>43092</v>
@@ -9277,7 +9310,7 @@
         <v>101</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="C103" s="4" t="s">
         <v>210</v>
@@ -9289,7 +9322,7 @@
         <v>54</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -9337,7 +9370,7 @@
         <v>104</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="C106" s="4">
         <v>2006</v>
@@ -9420,7 +9453,7 @@
         <v>54</v>
       </c>
       <c r="G110" s="43" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="111" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -9432,7 +9465,7 @@
         <v>222</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D111" s="19">
         <v>43319</v>
@@ -9450,7 +9483,7 @@
         <v>223</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="D112" s="19">
         <v>43327</v>
@@ -9459,7 +9492,7 @@
         <v>54</v>
       </c>
       <c r="G112" s="1" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="113" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -9471,7 +9504,7 @@
         <v>224</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="D113" s="19">
         <v>43346</v>
@@ -9489,7 +9522,7 @@
         <v>225</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="D114" s="19">
         <v>43353</v>
@@ -9501,7 +9534,7 @@
         <v>54</v>
       </c>
       <c r="G114" s="12" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="115" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -9513,7 +9546,7 @@
         <v>227</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="D115" s="19">
         <v>43373</v>
@@ -9531,7 +9564,7 @@
         <v>228</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="D116" s="19">
         <v>43375</v>
@@ -9561,7 +9594,7 @@
         <v>54</v>
       </c>
       <c r="G117" s="6" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="118" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -9690,7 +9723,7 @@
         <v>240</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="D124" s="19">
         <v>43470</v>
@@ -9705,10 +9738,10 @@
         <v>123</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="D125" s="19">
         <v>43513</v>
@@ -9747,7 +9780,7 @@
         <v>243</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="D127" s="19">
         <v>43582</v>
@@ -9765,7 +9798,7 @@
         <v>244</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="D128" s="19">
         <v>43590</v>
@@ -9783,7 +9816,7 @@
         <v>245</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="D129" s="19">
         <v>43617</v>
@@ -9798,16 +9831,16 @@
         <v>128</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="F130" s="1" t="s">
         <v>54</v>
       </c>
       <c r="G130" s="1" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="131" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -9847,7 +9880,7 @@
         <v>131</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="C133" s="4"/>
       <c r="F133" s="1" t="s">
@@ -10079,7 +10112,7 @@
         <v>148</v>
       </c>
       <c r="B150" s="24" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="C150" s="23"/>
       <c r="D150" s="20"/>
@@ -10087,7 +10120,7 @@
         <v>248</v>
       </c>
       <c r="G150" s="1" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="151" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -10096,7 +10129,7 @@
         <v>149</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="C151" s="4"/>
       <c r="F151" s="1" t="s">
@@ -10109,7 +10142,7 @@
         <v>150</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="C152" s="4"/>
       <c r="F152" s="1" t="s">
@@ -10122,7 +10155,7 @@
         <v>151</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="C153" s="4"/>
       <c r="F153" s="1" t="s">
@@ -10142,7 +10175,7 @@
         <v>248</v>
       </c>
       <c r="G154" s="12" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="155" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -10151,7 +10184,7 @@
         <v>153</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C155" s="4"/>
       <c r="F155" s="1" t="s">
@@ -10607,7 +10640,7 @@
         <v>307</v>
       </c>
       <c r="C189" s="4" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="D189" s="19">
         <v>42797</v>
@@ -10797,7 +10830,7 @@
         <v>331</v>
       </c>
       <c r="C203" s="4" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="D203" s="19">
         <v>42925</v>
@@ -10809,7 +10842,7 @@
         <v>332</v>
       </c>
       <c r="G203" s="1" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="204" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -10825,7 +10858,7 @@
         <v>334</v>
       </c>
       <c r="G204" s="1" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="205" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -10882,7 +10915,7 @@
         <v>206</v>
       </c>
       <c r="B208" s="8" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="C208" s="4"/>
       <c r="F208" s="1" t="s">
@@ -11111,14 +11144,14 @@
         <v>222</v>
       </c>
       <c r="B224" s="8" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="C224" s="4"/>
       <c r="F224" s="1" t="s">
         <v>370</v>
       </c>
       <c r="G224" s="1" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="225" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -11349,7 +11382,7 @@
         <v>238</v>
       </c>
       <c r="B240" s="24" t="s">
-        <v>1214</v>
+        <v>1212</v>
       </c>
       <c r="C240" s="23">
         <v>1997</v>
@@ -11436,14 +11469,14 @@
         <v>243</v>
       </c>
       <c r="B245" s="30" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="C245" s="4"/>
       <c r="D245" s="29" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="G245" s="12" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="246" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -11459,7 +11492,7 @@
         <v>370</v>
       </c>
       <c r="G246" s="1" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="247" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -11482,7 +11515,7 @@
       </c>
       <c r="C248" s="4"/>
       <c r="G248" s="1" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="249" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -11616,7 +11649,7 @@
         <v>258</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="C260" s="4"/>
       <c r="D260" s="19">
@@ -11690,13 +11723,13 @@
         <v>263</v>
       </c>
       <c r="B265" s="8" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="C265" s="4">
         <v>2007</v>
       </c>
       <c r="G265" s="12" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="266" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -11800,7 +11833,7 @@
         <v>271</v>
       </c>
       <c r="B273" s="24" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="C273" s="23"/>
       <c r="D273" s="20"/>
@@ -11887,7 +11920,7 @@
         <v>2008</v>
       </c>
       <c r="G280" s="1" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="281" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -12036,17 +12069,17 @@
     <row r="291" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A291" s="1"/>
       <c r="B291" s="8" t="s">
-        <v>1192</v>
+        <v>1190</v>
       </c>
       <c r="C291" s="4"/>
       <c r="D291" s="29" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
       <c r="E291" s="17" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="G291" s="1" t="s">
-        <v>1193</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="292" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -12055,7 +12088,7 @@
         <v>289</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>1215</v>
+        <v>1213</v>
       </c>
       <c r="C292" s="4">
         <v>2021</v>
@@ -12077,7 +12110,7 @@
       </c>
       <c r="C293" s="23"/>
       <c r="D293" s="21" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="G293" s="1" t="s">
         <v>470</v>
@@ -12089,7 +12122,7 @@
         <v>291</v>
       </c>
       <c r="B294" s="30" t="s">
-        <v>1206</v>
+        <v>1204</v>
       </c>
       <c r="C294" s="23"/>
       <c r="D294" s="20"/>
@@ -12100,7 +12133,7 @@
         <v>292</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>1207</v>
+        <v>1205</v>
       </c>
       <c r="C295" s="4">
         <v>2022</v>
@@ -12155,7 +12188,7 @@
         <v>295</v>
       </c>
       <c r="B298" s="1" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="C298" s="4"/>
     </row>
@@ -12171,10 +12204,10 @@
         <v>2021</v>
       </c>
       <c r="D299" s="21" t="s">
+        <v>1000</v>
+      </c>
+      <c r="G299" s="1" t="s">
         <v>1001</v>
-      </c>
-      <c r="G299" s="1" t="s">
-        <v>1002</v>
       </c>
     </row>
     <row r="300" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -12219,7 +12252,7 @@
         <v>298</v>
       </c>
       <c r="B302" s="1" t="s">
-        <v>1209</v>
+        <v>1207</v>
       </c>
       <c r="C302" s="4">
         <v>2022</v>
@@ -12248,7 +12281,7 @@
         <v>300</v>
       </c>
       <c r="B304" s="1" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="C304" s="4">
         <v>2017</v>
@@ -12260,7 +12293,7 @@
         <v>6.5</v>
       </c>
       <c r="G304" s="1" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="305" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -12268,7 +12301,7 @@
         <v>301</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
       <c r="C305" s="4">
         <v>2022</v>
@@ -12308,7 +12341,7 @@
         <v>303</v>
       </c>
       <c r="B307" s="1" t="s">
-        <v>1211</v>
+        <v>1209</v>
       </c>
       <c r="C307" s="4">
         <v>2001</v>
@@ -12328,13 +12361,13 @@
         <v>304</v>
       </c>
       <c r="B308" s="1" t="s">
-        <v>1210</v>
+        <v>1208</v>
       </c>
       <c r="C308" s="4">
         <v>2022</v>
       </c>
       <c r="D308" s="29" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="E308" s="16">
         <v>7.6</v>
@@ -12345,7 +12378,7 @@
         <v>305</v>
       </c>
       <c r="B309" s="30" t="s">
-        <v>1205</v>
+        <v>1203</v>
       </c>
       <c r="C309" s="4">
         <v>2023</v>
@@ -12362,7 +12395,7 @@
         <v>306</v>
       </c>
       <c r="B310" s="30" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="C310" s="28"/>
       <c r="D310" s="21">
@@ -12374,14 +12407,14 @@
         <v>307</v>
       </c>
       <c r="B311" s="24" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="C311" s="28"/>
       <c r="D311" s="21" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="G311" s="1" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="312" spans="1:7" x14ac:dyDescent="0.25">
@@ -12389,17 +12422,17 @@
         <v>308</v>
       </c>
       <c r="B312" s="24" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="C312" s="28"/>
       <c r="D312" s="21" t="s">
+        <v>1022</v>
+      </c>
+      <c r="E312" s="18" t="s">
+        <v>1024</v>
+      </c>
+      <c r="G312" s="6" t="s">
         <v>1023</v>
-      </c>
-      <c r="E312" s="18" t="s">
-        <v>1025</v>
-      </c>
-      <c r="G312" s="6" t="s">
-        <v>1024</v>
       </c>
     </row>
     <row r="313" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -12407,19 +12440,19 @@
         <v>309</v>
       </c>
       <c r="B313" s="25" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="C313" s="28">
         <v>2021</v>
       </c>
       <c r="D313" s="21" t="s">
+        <v>1025</v>
+      </c>
+      <c r="E313" s="17" t="s">
         <v>1026</v>
       </c>
-      <c r="E313" s="17" t="s">
+      <c r="G313" s="12" t="s">
         <v>1027</v>
-      </c>
-      <c r="G313" s="12" t="s">
-        <v>1028</v>
       </c>
     </row>
     <row r="314" spans="1:7" x14ac:dyDescent="0.25">
@@ -12427,14 +12460,14 @@
         <v>310</v>
       </c>
       <c r="B314" s="30" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="C314" s="28"/>
       <c r="D314" s="21" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="E314" s="17" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="315" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -12442,17 +12475,17 @@
         <v>311</v>
       </c>
       <c r="B315" s="24" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="C315" s="28"/>
       <c r="D315" s="21" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="E315" s="16">
         <v>5</v>
       </c>
       <c r="G315" s="12" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="316" spans="1:7" x14ac:dyDescent="0.25">
@@ -12460,11 +12493,11 @@
         <v>312</v>
       </c>
       <c r="B316" s="24" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="C316" s="28"/>
       <c r="D316" s="21" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="E316" s="16">
         <v>7</v>
@@ -12475,11 +12508,11 @@
         <v>313</v>
       </c>
       <c r="B317" s="26" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="C317" s="28"/>
       <c r="D317" s="21" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="318" spans="1:7" x14ac:dyDescent="0.25">
@@ -12487,19 +12520,19 @@
         <v>314</v>
       </c>
       <c r="B318" s="25" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="C318" s="28">
         <v>2021</v>
       </c>
       <c r="D318" s="21" t="s">
+        <v>1065</v>
+      </c>
+      <c r="E318" s="18" t="s">
         <v>1066</v>
       </c>
-      <c r="E318" s="18" t="s">
-        <v>1067</v>
-      </c>
       <c r="G318" s="12" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="319" spans="1:7" s="33" customFormat="1" x14ac:dyDescent="0.25">
@@ -12507,16 +12540,16 @@
         <v>315</v>
       </c>
       <c r="B319" s="33" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="C319" s="34">
         <v>2001</v>
       </c>
       <c r="D319" s="34" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="E319" s="35" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="G319" s="36"/>
     </row>
@@ -12525,14 +12558,14 @@
         <v>316</v>
       </c>
       <c r="B320" s="25" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="C320" s="4"/>
       <c r="D320" s="29" t="s">
+        <v>1112</v>
+      </c>
+      <c r="E320" s="18" t="s">
         <v>1113</v>
-      </c>
-      <c r="E320" s="18" t="s">
-        <v>1114</v>
       </c>
     </row>
     <row r="321" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -12540,17 +12573,17 @@
         <v>317</v>
       </c>
       <c r="B321" s="25" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="C321" s="4"/>
       <c r="D321" s="29" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="E321" s="18" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="G321" s="12" t="s">
-        <v>1182</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="322" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -12558,16 +12591,16 @@
         <v>318</v>
       </c>
       <c r="B322" s="24" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
       <c r="C322" s="4">
         <v>1988</v>
       </c>
       <c r="D322" s="29" t="s">
-        <v>1184</v>
+        <v>1182</v>
       </c>
       <c r="G322" s="6" t="s">
-        <v>1185</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="323" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -12575,17 +12608,17 @@
         <v>319</v>
       </c>
       <c r="B323" s="24" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="C323" s="4"/>
       <c r="D323" s="29" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="E323" s="18" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="G323" s="1" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="324" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -12593,14 +12626,14 @@
         <v>320</v>
       </c>
       <c r="B324" s="25" t="s">
-        <v>1204</v>
+        <v>1202</v>
       </c>
       <c r="C324" s="4"/>
       <c r="E324" s="48" t="s">
-        <v>1203</v>
+        <v>1201</v>
       </c>
       <c r="G324" s="1" t="s">
-        <v>1201</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="325" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -12608,17 +12641,17 @@
         <v>321</v>
       </c>
       <c r="B325" s="25" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
       <c r="C325" s="4"/>
       <c r="D325" s="29" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
       <c r="E325" s="48" t="s">
-        <v>1203</v>
+        <v>1201</v>
       </c>
       <c r="G325" s="1" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="326" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -12626,17 +12659,17 @@
         <v>322</v>
       </c>
       <c r="B326" s="25" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
       <c r="C326" s="4"/>
       <c r="D326" s="29" t="s">
-        <v>1220</v>
+        <v>1218</v>
       </c>
       <c r="E326" s="48" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="G326" s="1" t="s">
-        <v>1221</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="327" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -12644,16 +12677,16 @@
         <v>323</v>
       </c>
       <c r="B327" s="25" t="s">
-        <v>1224</v>
+        <v>1222</v>
       </c>
       <c r="D327" s="29" t="s">
-        <v>1219</v>
+        <v>1217</v>
       </c>
       <c r="E327" s="48" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
       <c r="G327" s="1" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="328" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -12661,16 +12694,16 @@
         <v>324</v>
       </c>
       <c r="B328" s="52" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="C328" s="4">
         <v>2015</v>
       </c>
       <c r="D328" s="29" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="E328" s="48" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="329" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -12678,19 +12711,19 @@
         <v>325</v>
       </c>
       <c r="B329" s="25" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="C329" s="4">
         <v>2000</v>
       </c>
       <c r="D329" s="29" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="E329" s="48" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="G329" s="1" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="330" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -14736,10 +14769,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H1005"/>
+  <dimension ref="A1:H1008"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14758,16 +14791,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>527</v>
+        <v>1263</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>528</v>
+        <v>1251</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>490</v>
@@ -14791,7 +14824,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="43" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="C3" s="39" t="s">
         <v>587</v>
@@ -14825,7 +14858,7 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -14917,7 +14950,7 @@
         <v>598</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>596</v>
+        <v>1262</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -14972,7 +15005,7 @@
         <v>604</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -15052,45 +15085,59 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="5" t="s">
-        <v>987</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>1</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1" t="s">
+        <v>1035</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>504</v>
+      </c>
+    </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1" t="s">
-        <v>1036</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>504</v>
+        <v>1035</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>507</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>506</v>
+        <v>509</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>507</v>
@@ -15098,159 +15145,156 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1" t="s">
-        <v>1036</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>507</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>510</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>511</v>
-      </c>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
+        <v>512</v>
+      </c>
       <c r="F30" s="1" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>1036</v>
+        <v>1035</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>514</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>1036</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>514</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>515</v>
-      </c>
+        <v>516</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
       <c r="F33" s="1" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1" t="s">
-        <v>1036</v>
+        <v>1035</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>520</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>518</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>519</v>
-      </c>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
+        <v>521</v>
+      </c>
       <c r="F35" s="1" t="s">
-        <v>1036</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>520</v>
+        <v>1035</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>507</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>521</v>
-      </c>
+        <v>522</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
       <c r="F36" s="1" t="s">
-        <v>1036</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>507</v>
+        <v>1035</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>522</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>523</v>
-      </c>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
+        <v>525</v>
+      </c>
       <c r="F37" s="1" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>524</v>
+        <v>526</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>507</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>525</v>
+        <v>1252</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>511</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>1036</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>526</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>507</v>
-      </c>
+        <v>1253</v>
+      </c>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
@@ -15266,139 +15310,165 @@
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
+    <row r="41" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="1" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>1051</v>
+      </c>
+      <c r="D41" s="1"/>
       <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
     </row>
     <row r="42" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
         <v>1030</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1052</v>
-      </c>
-      <c r="D42" s="1"/>
+        <v>1031</v>
+      </c>
+      <c r="D42" s="1">
+        <v>9</v>
+      </c>
+      <c r="E42" s="1">
+        <v>2023</v>
+      </c>
       <c r="F42" s="1"/>
     </row>
-    <row r="43" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>1031</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>1032</v>
-      </c>
-      <c r="D43" s="1">
-        <v>9</v>
-      </c>
-      <c r="E43" s="1">
-        <v>2023</v>
-      </c>
-      <c r="F43" s="1"/>
-    </row>
-    <row r="44" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="1" t="s">
-        <v>1039</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B45" s="12" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B44" s="12" t="s">
+        <v>1040</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>1041</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="D44" s="1"/>
+    </row>
+    <row r="45" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="1" t="s">
         <v>1042</v>
       </c>
-      <c r="D45" s="1"/>
     </row>
     <row r="46" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
-        <v>1043</v>
-      </c>
+        <v>1047</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D46" s="1"/>
     </row>
     <row r="47" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
-        <v>1048</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>1051</v>
-      </c>
-      <c r="D47" s="1"/>
+        <v>1058</v>
+      </c>
     </row>
     <row r="48" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="1" t="s">
-        <v>1059</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="14" t="s">
+        <v>1163</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="14" t="s">
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="32" t="s">
         <v>1164</v>
       </c>
     </row>
-    <row r="50" spans="2:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="14" t="s">
-        <v>1115</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="32" t="s">
         <v>1165</v>
       </c>
-    </row>
-    <row r="52" spans="2:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E51" s="1" t="s">
+        <v>1166</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="32" t="s">
-        <v>1166</v>
+        <v>1175</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>1167</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1254</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="32" t="s">
         <v>1176</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>1180</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="32" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>1257</v>
+      </c>
+      <c r="E54" s="1"/>
+    </row>
+    <row r="55" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="32" t="s">
+        <v>1260</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>1261</v>
+      </c>
+      <c r="E55" s="1"/>
+    </row>
+    <row r="56" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="32" t="s">
+        <v>1258</v>
+      </c>
+      <c r="C56" s="1"/>
+      <c r="E56" s="1" t="s">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="32"/>
+      <c r="C57" s="1"/>
+      <c r="E57" s="1"/>
+    </row>
+    <row r="58" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="32"/>
+      <c r="C58" s="1"/>
+      <c r="E58" s="1"/>
+    </row>
+    <row r="59" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="8" t="s">
         <v>1177</v>
       </c>
-      <c r="E54" s="1" t="s">
-        <v>1181</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="32"/>
-      <c r="E55" s="1"/>
-    </row>
-    <row r="56" spans="2:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="2:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="8" t="s">
-        <v>1178</v>
-      </c>
-    </row>
-    <row r="58" spans="2:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="1" t="s">
-        <v>991</v>
-      </c>
-    </row>
-    <row r="59" spans="2:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="2:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="2:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="2:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" spans="2:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="2:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="44" t="s">
-        <v>1179</v>
-      </c>
-    </row>
+    </row>
+    <row r="61" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="1" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="66" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="67" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="44" t="s">
+        <v>1178</v>
+      </c>
+    </row>
     <row r="69" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="70" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="71" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -16336,6 +16406,9 @@
     <row r="1003" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1004" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1005" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1006" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1007" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1008" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="5"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -16359,12 +16432,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>1186</v>
+        <v>1184</v>
       </c>
     </row>
   </sheetData>
@@ -16394,10 +16467,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>1045</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>1046</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>1047</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -16448,7 +16521,7 @@
         <v>496</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -16488,10 +16561,10 @@
     </row>
     <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
+        <v>1017</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>1018</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>1019</v>
       </c>
     </row>
     <row r="21" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -17990,37 +18063,37 @@
     <row r="53" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="54" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="8" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="8" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -19462,7 +19535,7 @@
         <v>617</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -19644,13 +19717,13 @@
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>663</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -23012,10 +23085,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>1045</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>1046</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>1047</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -24423,37 +24496,37 @@
     </row>
     <row r="13" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="18" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="19" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="20" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -24461,17 +24534,17 @@
     </row>
     <row r="21" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="6" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="22" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="23" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="24" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated watched and to-watch movies list
</commit_message>
<xml_diff>
--- a/thongnd_everything_list.xlsx
+++ b/thongnd_everything_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\ドキュメント\GitHub\My_Everything_Lists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBD7567-968E-4880-AF5A-DFB29AD08C24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52578B1C-D122-4515-B953-753FCDC2E1E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="885" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1_todolist" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
   <definedNames>
     <definedName name="beverage">beverage!$A$1:$B$11</definedName>
     <definedName name="game">'7_game'!$A$1:$C$31</definedName>
-    <definedName name="list_film_to_watch">'1_todolist'!$A$59:$D$108</definedName>
+    <definedName name="list_film_to_watch">'1_todolist'!$A$53:$D$102</definedName>
     <definedName name="music_list">'6_music_list'!$A$1:$D$296</definedName>
     <definedName name="reading_list">'3_book_list'!$A$1:$F$21</definedName>
     <definedName name="software_list">'5_software_list'!$A$1:$C$51</definedName>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1873" uniqueCount="1273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1891" uniqueCount="1291">
   <si>
     <t>ID</t>
   </si>
@@ -4388,32 +4388,6 @@
   <si>
     <r>
       <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ゴールデンカムイ　</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2024</t>
-    </r>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
         <sz val="11"/>
         <color rgb="FF00B050"/>
         <rFont val="Calibri"/>
@@ -4732,10 +4706,6 @@
   </si>
   <si>
     <t xml:space="preserve">Avatar </t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>Watched it when I was a little kid. Updated 2024.04.01</t>
     <phoneticPr fontId="5"/>
   </si>
   <si>
@@ -5222,10 +5192,6 @@
     <phoneticPr fontId="5"/>
   </si>
   <si>
-    <t>Steins Gate 0 (another series of Steins Gate)</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
     <t>保留中</t>
     <rPh sb="0" eb="3">
       <t>ホリュウチュウ</t>
@@ -5233,13 +5199,6 @@
     <phoneticPr fontId="5"/>
   </si>
   <si>
-    <t>新世紀エヴァンゲリオン</t>
-    <rPh sb="0" eb="3">
-      <t>シンセイキ</t>
-    </rPh>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
     <t>小林さんちのメイドラゴン</t>
     <rPh sb="0" eb="2">
       <t>コバヤシ</t>
@@ -5259,16 +5218,6 @@
   </si>
   <si>
     <t>https://myanimelist.net/anime/producer/2/Kyoto_Animation</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>探し方</t>
-    <rPh sb="0" eb="1">
-      <t>サガ</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>カタ</t>
-    </rPh>
     <phoneticPr fontId="5"/>
   </si>
   <si>
@@ -5382,10 +5331,6 @@
     <phoneticPr fontId="5"/>
   </si>
   <si>
-    <t>shougun.</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
     <t>STATUS</t>
     <phoneticPr fontId="5"/>
   </si>
@@ -5475,6 +5420,157 @@
   </si>
   <si>
     <t>I Wish I Could Meet You Again on the Hill Where That Flower Blooms</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>2024.11.01</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Neon Genesis Evangelion (全26話)</t>
+    <rPh sb="25" eb="26">
+      <t>ゼン</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>ワ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Steins;Gate 0</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Steins Gate with different world line</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Shougun (Season 1, 10 episodes)</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>2024.11.17</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>8.4/10</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="ＭＳ ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>ゴールデンカムイ　</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2024</t>
+    </r>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Brush Up Life</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Shitamachi Rocket</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>フルバージョンが見つけられない</t>
+    <rPh sb="8" eb="9">
+      <t>ミ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>不向き</t>
+    <rPh sb="0" eb="2">
+      <t>フム</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>探し方。日本の人気のある映画評価サイト</t>
+    <rPh sb="0" eb="1">
+      <t>サガ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>カタ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ニホン</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ニンキ</t>
+    </rPh>
+    <rPh sb="12" eb="16">
+      <t>エイガヒョウカ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>https://eiga.com/drama/series/shogun/review/6/</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Mathematic, Genius</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>8.5/10</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Watched it when I was a little kid with my cousins. Updated 2024.04.01</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>True Detective</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Deadpool &amp; Wolverine</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>2024.11.30</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>6.8/10</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Venom 2024. 
+評価が低いので、スキップする</t>
+    <rPh sb="13" eb="15">
+      <t>ヒョウカ</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>ヒク</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>America Psycho　-&gt; skip</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Arrival 2016</t>
     <phoneticPr fontId="5"/>
   </si>
 </sst>
@@ -5482,7 +5578,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5563,14 +5659,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Meiryo UI"/>
-      <family val="3"/>
-      <charset val="128"/>
     </font>
     <font>
       <sz val="11"/>
@@ -5715,6 +5803,21 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="ＭＳ ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -5749,7 +5852,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5773,8 +5876,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5796,13 +5898,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -5812,22 +5914,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="56" fontId="20" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="56" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -5844,25 +5946,33 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8"/>
@@ -6079,603 +6189,616 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1043"/>
+  <dimension ref="A1:D1037"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.7109375" customWidth="1"/>
     <col min="2" max="2" width="88.42578125" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" customWidth="1"/>
+    <col min="3" max="3" width="59.140625" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="50" t="s">
-        <v>1230</v>
+      <c r="B1" s="49" t="s">
+        <v>1226</v>
       </c>
     </row>
     <row r="2" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="48" t="s">
+        <v>1224</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="48" t="s">
+        <v>1284</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="48"/>
+    </row>
+    <row r="8" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="43" t="s">
+        <v>1145</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="52" t="s">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="23" t="s">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="48" t="s">
         <v>1225</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="22" t="s">
+    <row r="12" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="23"/>
+    </row>
+    <row r="13" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="48" t="s">
+        <v>1279</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="10" t="s">
         <v>1227</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="49" t="s">
-        <v>1228</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="49" t="s">
-        <v>1249</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="49"/>
-    </row>
-    <row r="8" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="44" t="s">
-        <v>1145</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>1166</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="30" t="s">
-        <v>1159</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="24" t="s">
-        <v>1157</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="49" t="s">
-        <v>1229</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="24"/>
-    </row>
-    <row r="13" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="24"/>
-    </row>
-    <row r="14" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="49" t="s">
-        <v>1232</v>
       </c>
     </row>
     <row r="15" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
-        <v>1231</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="16" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="10" t="s">
-        <v>1234</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
-        <v>1235</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="18" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="10"/>
     </row>
     <row r="19" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="10"/>
+      <c r="B19" s="1"/>
     </row>
     <row r="20" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
+      <c r="B20" s="49" t="s">
+        <v>1223</v>
+      </c>
     </row>
     <row r="21" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="50" t="s">
-        <v>1226</v>
+      <c r="B21" s="11" t="s">
+        <v>1062</v>
       </c>
     </row>
     <row r="22" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="11" t="s">
-        <v>1062</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>1061</v>
       </c>
     </row>
+    <row r="23" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="11" t="s">
+        <v>988</v>
+      </c>
+    </row>
     <row r="24" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="13"/>
+      <c r="B24" s="1" t="s">
+        <v>1012</v>
+      </c>
     </row>
     <row r="25" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="11" t="s">
-        <v>988</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="B25" s="21" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
     <row r="27" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>1012</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="28" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="22" t="s">
-        <v>1060</v>
-      </c>
-    </row>
-    <row r="29" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="B28" s="1" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>1010</v>
+      </c>
+    </row>
     <row r="30" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>39</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="31" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="32" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>1014</v>
+      </c>
+    </row>
     <row r="33" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="1" t="s">
-        <v>1009</v>
+      <c r="B33" s="6" t="s">
+        <v>1167</v>
       </c>
     </row>
     <row r="34" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="1" t="s">
-        <v>1010</v>
+      <c r="B34" s="6" t="s">
+        <v>1122</v>
       </c>
     </row>
     <row r="35" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="1"/>
+      <c r="B35" s="1" t="s">
+        <v>1126</v>
+      </c>
     </row>
     <row r="36" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="1" t="s">
-        <v>1011</v>
+      <c r="B36" s="6" t="s">
+        <v>1121</v>
       </c>
     </row>
     <row r="37" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>1013</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="38" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="1" t="s">
-        <v>1014</v>
+      <c r="B38" s="6" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>1166</v>
       </c>
     </row>
     <row r="39" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="6" t="s">
-        <v>1168</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="6" t="s">
-        <v>1122</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="1"/>
+    </row>
+    <row r="40" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="8" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
-        <v>1126</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="6" t="s">
-        <v>1121</v>
-      </c>
-    </row>
-    <row r="43" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="1" t="s">
-        <v>1018</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="6" t="s">
-        <v>1224</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>1167</v>
-      </c>
+        <v>1124</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="1" t="s">
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="1"/>
+    </row>
+    <row r="44" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="8"/>
     </row>
     <row r="45" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="1"/>
-    </row>
-    <row r="46" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="8" t="s">
-        <v>1123</v>
-      </c>
-    </row>
-    <row r="47" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="37" t="s">
+        <v>1138</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="1" t="s">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
-        <v>1124</v>
-      </c>
-    </row>
-    <row r="48" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
-        <v>1125</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="1"/>
-    </row>
-    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="8"/>
-    </row>
-    <row r="51" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="38" t="s">
-        <v>1138</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="1" t="s">
-        <v>1105</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="8"/>
+    </row>
+    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="43" t="s">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B53" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>1</v>
+      </c>
       <c r="B54" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>986</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="8"/>
-    </row>
-    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="44" t="s">
-        <v>1146</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C59" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <f t="shared" ref="A55:A57" si="0">A54+1</f>
         <v>2</v>
       </c>
-      <c r="D59" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="1">
-        <v>1</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="1">
-        <f t="shared" ref="A61:A63" si="0">A60+1</f>
-        <v>2</v>
-      </c>
-      <c r="B61" s="1" t="s">
+      <c r="B55" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C55" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="1">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B56" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D62" s="1" t="s">
+      <c r="D56" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="1">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
+      <c r="B57" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B58" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B59" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B60" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B61" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B62" s="1" t="s">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B63" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B64" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
-        <v>1155</v>
+        <v>22</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69" s="1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B72" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B72" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="78" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B78" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B78" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="79" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="80" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="81" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
     <row r="82" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="B82" s="1"/>
     </row>
     <row r="83" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="84" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
+      <c r="B83" s="1"/>
+    </row>
+    <row r="84" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="85" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="1" t="s">
-        <v>35</v>
+      <c r="B85" s="3" t="s">
+        <v>1221</v>
       </c>
     </row>
     <row r="86" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="87" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="88" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="1"/>
-    </row>
-    <row r="89" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B89" s="1"/>
-    </row>
+      <c r="B88" t="s">
+        <v>1172</v>
+      </c>
+    </row>
+    <row r="89" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="90" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="91" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" s="3" t="s">
-        <v>1223</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="92" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="93" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="94" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B94" t="s">
-        <v>1173</v>
-      </c>
-    </row>
-    <row r="95" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="96" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="B94" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="95" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B95" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="96" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B96" s="1" t="s">
+        <v>987</v>
+      </c>
+    </row>
     <row r="97" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B97" s="3" t="s">
-        <v>1106</v>
+      <c r="B97" s="6" t="s">
+        <v>1008</v>
       </c>
     </row>
     <row r="98" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B98" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>43</v>
+      <c r="B98" s="6" t="s">
+        <v>1019</v>
       </c>
     </row>
     <row r="99" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B99" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="100" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B100" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="101" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B101" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="102" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B102" s="1" t="s">
-        <v>987</v>
+      <c r="B99" s="6" t="s">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="101" spans="2:3" ht="55.5" x14ac:dyDescent="0.25">
+      <c r="B101" s="36" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C101" s="50" t="s">
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="102" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B102" s="6" t="s">
+        <v>1168</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>1169</v>
       </c>
     </row>
     <row r="103" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B103" s="6" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="104" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B104" s="6" t="s">
-        <v>1019</v>
-      </c>
-    </row>
-    <row r="105" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1020</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="105" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B105" s="6" t="s">
-        <v>1104</v>
-      </c>
-    </row>
-    <row r="107" spans="2:3" ht="55.5" x14ac:dyDescent="0.25">
-      <c r="B107" s="37" t="s">
-        <v>1053</v>
-      </c>
-      <c r="C107" s="51" t="s">
-        <v>1233</v>
-      </c>
-    </row>
-    <row r="108" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B108" s="6" t="s">
-        <v>1169</v>
-      </c>
-      <c r="C108" s="5" t="s">
-        <v>1170</v>
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="106" spans="2:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="B106" s="53" t="s">
+        <v>1159</v>
+      </c>
+      <c r="C106" s="44" t="s">
+        <v>1171</v>
+      </c>
+    </row>
+    <row r="107" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B107" s="1" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="108" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B108" s="1" t="s">
+        <v>1275</v>
+      </c>
+      <c r="C108" s="54" t="s">
+        <v>1278</v>
       </c>
     </row>
     <row r="109" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B109" s="6" t="s">
-        <v>1007</v>
+      <c r="B109" s="1" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>1277</v>
       </c>
     </row>
     <row r="110" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B110" s="6" t="s">
-        <v>1020</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>1186</v>
-      </c>
-    </row>
-    <row r="111" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B111" s="6" t="s">
-        <v>1185</v>
-      </c>
-    </row>
-    <row r="112" spans="2:3" ht="64.5" x14ac:dyDescent="0.25">
-      <c r="B112" s="24" t="s">
-        <v>1160</v>
-      </c>
-      <c r="C112" s="45" t="s">
-        <v>1172</v>
-      </c>
-    </row>
-    <row r="113" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B113" s="1" t="s">
-        <v>1006</v>
-      </c>
-    </row>
-    <row r="114" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="115" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="116" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="117" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="118" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="119" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="120" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="121" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="124" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="125" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="126" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="127" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="128" spans="2:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="B110" s="55" t="s">
+        <v>1288</v>
+      </c>
+    </row>
+    <row r="111" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B111" s="21" t="s">
+        <v>1289</v>
+      </c>
+    </row>
+    <row r="112" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="129" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="130" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="131" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7585,30 +7708,25 @@
     <row r="1035" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1036" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1037" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1038" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1039" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1040" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1041" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1042" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1043" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="5"/>
   <hyperlinks>
-    <hyperlink ref="B15" r:id="rId1" xr:uid="{84274C41-67A4-4C42-A214-2B8352868740}"/>
-    <hyperlink ref="B16" r:id="rId2" xr:uid="{EC16E6DB-BF4A-4A9B-93C6-121FD5F6D83E}"/>
-    <hyperlink ref="B17" r:id="rId3" xr:uid="{FF4AF8CB-4606-4702-B590-B95074E1C7F2}"/>
+    <hyperlink ref="B14" r:id="rId1" xr:uid="{84274C41-67A4-4C42-A214-2B8352868740}"/>
+    <hyperlink ref="B15" r:id="rId2" xr:uid="{EC16E6DB-BF4A-4A9B-93C6-121FD5F6D83E}"/>
+    <hyperlink ref="B16" r:id="rId3" xr:uid="{FF4AF8CB-4606-4702-B590-B95074E1C7F2}"/>
+    <hyperlink ref="B17" r:id="rId4" xr:uid="{B5CE4C32-7354-48AA-AA4F-F2B635E7F675}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G1007"/>
+  <dimension ref="A1:G1008"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A315" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B329" sqref="B329"/>
+    <sheetView tabSelected="1" topLeftCell="A322" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B153" sqref="B153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7616,8 +7734,8 @@
     <col min="1" max="1" width="7.5703125" customWidth="1"/>
     <col min="2" max="2" width="69.28515625" customWidth="1"/>
     <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="68.28515625" style="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="16" customWidth="1"/>
+    <col min="4" max="4" width="68.28515625" style="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="15" customWidth="1"/>
     <col min="6" max="6" width="13.7109375" customWidth="1"/>
     <col min="7" max="7" width="69.28515625" customWidth="1"/>
     <col min="8" max="26" width="8.7109375" customWidth="1"/>
@@ -7633,10 +7751,10 @@
       <c r="C1" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="14" t="s">
         <v>51</v>
       </c>
       <c r="F1" s="8" t="s">
@@ -7764,7 +7882,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="C11" s="4"/>
       <c r="F11" s="1" t="s">
@@ -7806,7 +7924,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>1214</v>
+        <v>1212</v>
       </c>
       <c r="C14" s="4"/>
       <c r="F14" s="1" t="s">
@@ -7845,7 +7963,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>1215</v>
+        <v>1213</v>
       </c>
       <c r="C17" s="4"/>
       <c r="F17" s="1" t="s">
@@ -7996,6 +8114,9 @@
         <v>1151</v>
       </c>
       <c r="C29" s="4"/>
+      <c r="E29" s="16" t="s">
+        <v>1282</v>
+      </c>
       <c r="F29" s="1" t="s">
         <v>54</v>
       </c>
@@ -8073,7 +8194,7 @@
         <v>89</v>
       </c>
       <c r="C35" s="4"/>
-      <c r="D35" s="19">
+      <c r="D35" s="18">
         <v>40337</v>
       </c>
       <c r="F35" s="1" t="s">
@@ -8124,7 +8245,7 @@
         <v>93</v>
       </c>
       <c r="C39" s="4"/>
-      <c r="D39" s="19">
+      <c r="D39" s="18">
         <v>42366</v>
       </c>
       <c r="F39" s="1" t="s">
@@ -8139,7 +8260,7 @@
         <v>94</v>
       </c>
       <c r="C40" s="4"/>
-      <c r="D40" s="19">
+      <c r="D40" s="18">
         <v>42422</v>
       </c>
       <c r="F40" s="1" t="s">
@@ -8154,7 +8275,7 @@
         <v>1153</v>
       </c>
       <c r="C41" s="4"/>
-      <c r="D41" s="19">
+      <c r="D41" s="18">
         <v>42481</v>
       </c>
       <c r="F41" s="1" t="s">
@@ -8171,7 +8292,7 @@
       <c r="C42" s="4" t="s">
         <v>1079</v>
       </c>
-      <c r="D42" s="19">
+      <c r="D42" s="18">
         <v>42499</v>
       </c>
       <c r="F42" s="1" t="s">
@@ -8186,7 +8307,7 @@
         <v>96</v>
       </c>
       <c r="C43" s="4"/>
-      <c r="D43" s="19">
+      <c r="D43" s="18">
         <v>42526</v>
       </c>
       <c r="F43" s="1" t="s">
@@ -8201,7 +8322,7 @@
         <v>97</v>
       </c>
       <c r="C44" s="4"/>
-      <c r="D44" s="19">
+      <c r="D44" s="18">
         <v>42530</v>
       </c>
       <c r="F44" s="1" t="s">
@@ -8258,7 +8379,7 @@
       <c r="C48" s="4" t="s">
         <v>1077</v>
       </c>
-      <c r="E48" s="17" t="s">
+      <c r="E48" s="16" t="s">
         <v>102</v>
       </c>
       <c r="F48" s="1" t="s">
@@ -8285,10 +8406,10 @@
         <v>104</v>
       </c>
       <c r="C50" s="4"/>
-      <c r="D50" s="19">
+      <c r="D50" s="18">
         <v>42576</v>
       </c>
-      <c r="E50" s="17" t="s">
+      <c r="E50" s="16" t="s">
         <v>105</v>
       </c>
       <c r="F50" s="1" t="s">
@@ -8303,10 +8424,10 @@
         <v>106</v>
       </c>
       <c r="C51" s="4"/>
-      <c r="D51" s="19">
+      <c r="D51" s="18">
         <v>42579</v>
       </c>
-      <c r="E51" s="17" t="s">
+      <c r="E51" s="16" t="s">
         <v>107</v>
       </c>
       <c r="F51" s="1" t="s">
@@ -8326,10 +8447,10 @@
       <c r="C52" s="4" t="s">
         <v>1080</v>
       </c>
-      <c r="D52" s="19">
+      <c r="D52" s="18">
         <v>42468</v>
       </c>
-      <c r="E52" s="17" t="s">
+      <c r="E52" s="16" t="s">
         <v>110</v>
       </c>
       <c r="F52" s="1" t="s">
@@ -8346,10 +8467,10 @@
       <c r="C53" s="4" t="s">
         <v>1081</v>
       </c>
-      <c r="D53" s="19">
+      <c r="D53" s="18">
         <v>42498</v>
       </c>
-      <c r="E53" s="17" t="s">
+      <c r="E53" s="16" t="s">
         <v>112</v>
       </c>
       <c r="F53" s="1" t="s">
@@ -8366,10 +8487,10 @@
       <c r="C54" s="4" t="s">
         <v>1082</v>
       </c>
-      <c r="D54" s="19">
+      <c r="D54" s="18">
         <v>42529</v>
       </c>
-      <c r="E54" s="17" t="s">
+      <c r="E54" s="16" t="s">
         <v>114</v>
       </c>
       <c r="F54" s="1" t="s">
@@ -8386,10 +8507,10 @@
       <c r="C55" s="4">
         <v>1990</v>
       </c>
-      <c r="D55" s="19">
+      <c r="D55" s="18">
         <v>42651</v>
       </c>
-      <c r="E55" s="17" t="s">
+      <c r="E55" s="16" t="s">
         <v>114</v>
       </c>
       <c r="F55" s="1" t="s">
@@ -8406,10 +8527,10 @@
       <c r="C56" s="4">
         <v>2011</v>
       </c>
-      <c r="D56" s="19">
+      <c r="D56" s="18">
         <v>42682</v>
       </c>
-      <c r="E56" s="17" t="s">
+      <c r="E56" s="16" t="s">
         <v>117</v>
       </c>
       <c r="F56" s="1" t="s">
@@ -8429,10 +8550,10 @@
       <c r="C57" s="4" t="s">
         <v>1082</v>
       </c>
-      <c r="D57" s="19">
+      <c r="D57" s="18">
         <v>42712</v>
       </c>
-      <c r="E57" s="17" t="s">
+      <c r="E57" s="16" t="s">
         <v>120</v>
       </c>
       <c r="F57" s="1" t="s">
@@ -8452,7 +8573,7 @@
       <c r="C58" s="4" t="s">
         <v>1082</v>
       </c>
-      <c r="D58" s="19">
+      <c r="D58" s="18">
         <v>42605</v>
       </c>
       <c r="F58" s="1" t="s">
@@ -8469,10 +8590,10 @@
       <c r="C59" s="4" t="s">
         <v>1083</v>
       </c>
-      <c r="D59" s="19">
+      <c r="D59" s="18">
         <v>42560</v>
       </c>
-      <c r="E59" s="17" t="s">
+      <c r="E59" s="16" t="s">
         <v>124</v>
       </c>
       <c r="F59" s="1" t="s">
@@ -8489,10 +8610,10 @@
       <c r="C60" s="4">
         <v>2002</v>
       </c>
-      <c r="D60" s="19">
+      <c r="D60" s="18">
         <v>42628</v>
       </c>
-      <c r="E60" s="17" t="s">
+      <c r="E60" s="16" t="s">
         <v>126</v>
       </c>
       <c r="F60" s="1" t="s">
@@ -8512,10 +8633,10 @@
       <c r="C61" s="4" t="s">
         <v>1084</v>
       </c>
-      <c r="D61" s="19">
+      <c r="D61" s="18">
         <v>42665</v>
       </c>
-      <c r="E61" s="17" t="s">
+      <c r="E61" s="16" t="s">
         <v>129</v>
       </c>
       <c r="F61" s="1" t="s">
@@ -8542,10 +8663,10 @@
         <v>131</v>
       </c>
       <c r="C63" s="4"/>
-      <c r="D63" s="19">
+      <c r="D63" s="18">
         <v>42751</v>
       </c>
-      <c r="E63" s="17" t="s">
+      <c r="E63" s="16" t="s">
         <v>132</v>
       </c>
       <c r="F63" s="1" t="s">
@@ -8560,7 +8681,7 @@
         <v>133</v>
       </c>
       <c r="C64" s="4"/>
-      <c r="D64" s="19">
+      <c r="D64" s="18">
         <v>42753</v>
       </c>
       <c r="F64" s="1" t="s">
@@ -8577,10 +8698,10 @@
       <c r="C65" s="4" t="s">
         <v>1082</v>
       </c>
-      <c r="D65" s="19">
+      <c r="D65" s="18">
         <v>42756</v>
       </c>
-      <c r="E65" s="17" t="s">
+      <c r="E65" s="16" t="s">
         <v>135</v>
       </c>
       <c r="F65" s="1" t="s">
@@ -8595,7 +8716,7 @@
         <v>136</v>
       </c>
       <c r="C66" s="4"/>
-      <c r="D66" s="19">
+      <c r="D66" s="18">
         <v>42756</v>
       </c>
       <c r="F66" s="1" t="s">
@@ -8615,10 +8736,10 @@
       <c r="C67" s="4" t="s">
         <v>1098</v>
       </c>
-      <c r="D67" s="19">
+      <c r="D67" s="18">
         <v>42757</v>
       </c>
-      <c r="E67" s="17" t="s">
+      <c r="E67" s="16" t="s">
         <v>110</v>
       </c>
       <c r="F67" s="1" t="s">
@@ -8635,10 +8756,10 @@
       <c r="C68" s="4">
         <v>2010</v>
       </c>
-      <c r="D68" s="19">
+      <c r="D68" s="18">
         <v>42758</v>
       </c>
-      <c r="E68" s="17" t="s">
+      <c r="E68" s="16" t="s">
         <v>140</v>
       </c>
       <c r="F68" s="1" t="s">
@@ -8655,10 +8776,10 @@
       <c r="C69" s="4">
         <v>2016</v>
       </c>
-      <c r="D69" s="19">
+      <c r="D69" s="18">
         <v>42765</v>
       </c>
-      <c r="E69" s="17" t="s">
+      <c r="E69" s="16" t="s">
         <v>142</v>
       </c>
       <c r="F69" s="1" t="s">
@@ -8675,10 +8796,10 @@
       <c r="C70" s="4">
         <v>1995</v>
       </c>
-      <c r="D70" s="19">
+      <c r="D70" s="18">
         <v>42768</v>
       </c>
-      <c r="E70" s="17" t="s">
+      <c r="E70" s="16" t="s">
         <v>144</v>
       </c>
       <c r="F70" s="1" t="s">
@@ -8695,7 +8816,7 @@
       <c r="C71" s="4">
         <v>1987</v>
       </c>
-      <c r="D71" s="19">
+      <c r="D71" s="18">
         <v>42829</v>
       </c>
       <c r="F71" s="1" t="s">
@@ -8715,10 +8836,10 @@
       <c r="C72" s="4" t="s">
         <v>1085</v>
       </c>
-      <c r="D72" s="19">
+      <c r="D72" s="18">
         <v>42838</v>
       </c>
-      <c r="E72" s="17" t="s">
+      <c r="E72" s="16" t="s">
         <v>1149</v>
       </c>
       <c r="F72" s="1" t="s">
@@ -8735,10 +8856,10 @@
       <c r="C73" s="4" t="s">
         <v>1086</v>
       </c>
-      <c r="D73" s="19">
+      <c r="D73" s="18">
         <v>42963</v>
       </c>
-      <c r="E73" s="17" t="s">
+      <c r="E73" s="16" t="s">
         <v>149</v>
       </c>
       <c r="F73" s="1" t="s">
@@ -8758,10 +8879,10 @@
       <c r="C74" s="4" t="s">
         <v>1087</v>
       </c>
-      <c r="D74" s="19">
+      <c r="D74" s="18">
         <v>42980</v>
       </c>
-      <c r="E74" s="17" t="s">
+      <c r="E74" s="16" t="s">
         <v>152</v>
       </c>
       <c r="F74" s="1" t="s">
@@ -8778,10 +8899,10 @@
       <c r="C75" s="4" t="s">
         <v>1087</v>
       </c>
-      <c r="D75" s="19">
+      <c r="D75" s="18">
         <v>43007</v>
       </c>
-      <c r="E75" s="17" t="s">
+      <c r="E75" s="16" t="s">
         <v>154</v>
       </c>
       <c r="F75" s="1" t="s">
@@ -8798,27 +8919,27 @@
       <c r="C76" s="4" t="s">
         <v>1086</v>
       </c>
-      <c r="D76" s="19">
+      <c r="D76" s="18">
         <v>43019</v>
       </c>
-      <c r="E76" s="17" t="s">
+      <c r="E76" s="16" t="s">
         <v>149</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="77" spans="1:7" s="33" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="33" t="s">
-        <v>1187</v>
-      </c>
-      <c r="C77" s="46">
+    <row r="77" spans="1:7" s="32" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B77" s="32" t="s">
+        <v>1186</v>
+      </c>
+      <c r="C77" s="45">
         <v>2009</v>
       </c>
-      <c r="D77" s="34"/>
-      <c r="E77" s="47"/>
-      <c r="G77" s="33" t="s">
-        <v>1188</v>
+      <c r="D77" s="33"/>
+      <c r="E77" s="46"/>
+      <c r="G77" s="32" t="s">
+        <v>1283</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -8830,7 +8951,7 @@
         <v>156</v>
       </c>
       <c r="C78" s="4"/>
-      <c r="D78" s="19">
+      <c r="D78" s="18">
         <v>43043</v>
       </c>
       <c r="F78" s="1" t="s">
@@ -8863,10 +8984,10 @@
       <c r="C80" s="4">
         <v>2017</v>
       </c>
-      <c r="D80" s="19">
+      <c r="D80" s="18">
         <v>43072</v>
       </c>
-      <c r="E80" s="17" t="s">
+      <c r="E80" s="16" t="s">
         <v>160</v>
       </c>
       <c r="F80" s="1" t="s">
@@ -8884,10 +9005,10 @@
       <c r="C81" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="D81" s="19">
+      <c r="D81" s="18">
         <v>43076</v>
       </c>
-      <c r="E81" s="17" t="s">
+      <c r="E81" s="16" t="s">
         <v>149</v>
       </c>
       <c r="F81" s="1" t="s">
@@ -8908,10 +9029,10 @@
       <c r="C82" s="4">
         <v>2009</v>
       </c>
-      <c r="D82" s="19">
+      <c r="D82" s="18">
         <v>43086</v>
       </c>
-      <c r="E82" s="17" t="s">
+      <c r="E82" s="16" t="s">
         <v>110</v>
       </c>
       <c r="F82" s="1" t="s">
@@ -8929,10 +9050,10 @@
       <c r="C83" s="4">
         <v>2001</v>
       </c>
-      <c r="D83" s="31">
+      <c r="D83" s="30">
         <v>43090</v>
       </c>
-      <c r="E83" s="17" t="s">
+      <c r="E83" s="16" t="s">
         <v>149</v>
       </c>
       <c r="F83" s="1" t="s">
@@ -8953,10 +9074,10 @@
       <c r="C84" s="4" t="s">
         <v>1085</v>
       </c>
-      <c r="D84" s="19">
+      <c r="D84" s="18">
         <v>43092</v>
       </c>
-      <c r="E84" s="17" t="s">
+      <c r="E84" s="16" t="s">
         <v>142</v>
       </c>
       <c r="F84" s="1" t="s">
@@ -8975,7 +9096,7 @@
         <v>168</v>
       </c>
       <c r="C85" s="4"/>
-      <c r="D85" s="19">
+      <c r="D85" s="18">
         <v>43070</v>
       </c>
       <c r="F85" s="1" t="s">
@@ -8996,10 +9117,10 @@
       <c r="C86" s="4">
         <v>2017</v>
       </c>
-      <c r="D86" s="19">
+      <c r="D86" s="18">
         <v>43096</v>
       </c>
-      <c r="E86" s="17" t="s">
+      <c r="E86" s="16" t="s">
         <v>171</v>
       </c>
       <c r="F86" s="1" t="s">
@@ -9031,7 +9152,7 @@
         <v>174</v>
       </c>
       <c r="C88" s="4"/>
-      <c r="E88" s="17" t="s">
+      <c r="E88" s="16" t="s">
         <v>175</v>
       </c>
       <c r="F88" s="1" t="s">
@@ -9052,10 +9173,10 @@
       <c r="C89" s="4">
         <v>2017</v>
       </c>
-      <c r="D89" s="19">
+      <c r="D89" s="18">
         <v>43111</v>
       </c>
-      <c r="E89" s="17" t="s">
+      <c r="E89" s="16" t="s">
         <v>178</v>
       </c>
       <c r="F89" s="1" t="s">
@@ -9074,7 +9195,7 @@
         <v>180</v>
       </c>
       <c r="C90" s="4"/>
-      <c r="D90" s="19">
+      <c r="D90" s="18">
         <v>43127</v>
       </c>
       <c r="F90" s="1" t="s">
@@ -9093,10 +9214,10 @@
         <v>182</v>
       </c>
       <c r="C91" s="4"/>
-      <c r="D91" s="19">
+      <c r="D91" s="18">
         <v>43137</v>
       </c>
-      <c r="E91" s="17" t="s">
+      <c r="E91" s="16" t="s">
         <v>183</v>
       </c>
       <c r="F91" s="1" t="s">
@@ -9112,7 +9233,7 @@
         <v>184</v>
       </c>
       <c r="C92" s="4"/>
-      <c r="D92" s="19">
+      <c r="D92" s="18">
         <v>43138</v>
       </c>
       <c r="F92" s="1" t="s">
@@ -9133,10 +9254,10 @@
       <c r="C93" s="4">
         <v>2017</v>
       </c>
-      <c r="D93" s="19">
+      <c r="D93" s="18">
         <v>43177</v>
       </c>
-      <c r="E93" s="17" t="s">
+      <c r="E93" s="16" t="s">
         <v>187</v>
       </c>
       <c r="F93" s="1" t="s">
@@ -9154,10 +9275,10 @@
       <c r="C94" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="D94" s="19">
+      <c r="D94" s="18">
         <v>43194</v>
       </c>
-      <c r="E94" s="17" t="s">
+      <c r="E94" s="16" t="s">
         <v>190</v>
       </c>
       <c r="F94" s="1" t="s">
@@ -9178,10 +9299,10 @@
       <c r="C95" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="D95" s="19">
+      <c r="D95" s="18">
         <v>43204</v>
       </c>
-      <c r="E95" s="17" t="s">
+      <c r="E95" s="16" t="s">
         <v>194</v>
       </c>
       <c r="F95" s="1" t="s">
@@ -9199,10 +9320,10 @@
       <c r="C96" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="D96" s="19">
+      <c r="D96" s="18">
         <v>43230</v>
       </c>
-      <c r="E96" s="17" t="s">
+      <c r="E96" s="16" t="s">
         <v>152</v>
       </c>
       <c r="F96" s="1" t="s">
@@ -9223,10 +9344,10 @@
       <c r="C97" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="D97" s="19">
+      <c r="D97" s="18">
         <v>43252</v>
       </c>
-      <c r="E97" s="17" t="s">
+      <c r="E97" s="16" t="s">
         <v>154</v>
       </c>
       <c r="F97" s="1" t="s">
@@ -9247,10 +9368,10 @@
       <c r="C98" s="4">
         <v>1999</v>
       </c>
-      <c r="D98" s="19">
+      <c r="D98" s="18">
         <v>43253</v>
       </c>
-      <c r="E98" s="17" t="s">
+      <c r="E98" s="16" t="s">
         <v>201</v>
       </c>
       <c r="F98" s="1" t="s">
@@ -9268,7 +9389,7 @@
       <c r="C99" s="4">
         <v>2018</v>
       </c>
-      <c r="E99" s="17" t="s">
+      <c r="E99" s="16" t="s">
         <v>194</v>
       </c>
       <c r="F99" s="1" t="s">
@@ -9286,7 +9407,7 @@
       <c r="C100" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="D100" s="19">
+      <c r="D100" s="18">
         <v>43290</v>
       </c>
       <c r="F100" s="1" t="s">
@@ -9307,10 +9428,10 @@
       <c r="C101" s="4">
         <v>2018</v>
       </c>
-      <c r="D101" s="19">
+      <c r="D101" s="18">
         <v>43291</v>
       </c>
-      <c r="E101" s="17" t="s">
+      <c r="E101" s="16" t="s">
         <v>194</v>
       </c>
       <c r="F101" s="1" t="s">
@@ -9331,10 +9452,10 @@
       <c r="C102" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="D102" s="19">
+      <c r="D102" s="18">
         <v>43297</v>
       </c>
-      <c r="E102" s="17" t="s">
+      <c r="E102" s="16" t="s">
         <v>209</v>
       </c>
       <c r="F102" s="1" t="s">
@@ -9352,7 +9473,7 @@
       <c r="C103" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="D103" s="19">
+      <c r="D103" s="18">
         <v>43303</v>
       </c>
       <c r="F103" s="1" t="s">
@@ -9391,7 +9512,7 @@
       <c r="C105" s="4">
         <v>2004</v>
       </c>
-      <c r="D105" s="19">
+      <c r="D105" s="18">
         <v>43302</v>
       </c>
       <c r="F105" s="1" t="s">
@@ -9412,7 +9533,7 @@
       <c r="C106" s="4">
         <v>2006</v>
       </c>
-      <c r="D106" s="19">
+      <c r="D106" s="18">
         <v>43304</v>
       </c>
       <c r="F106" s="1" t="s">
@@ -9430,7 +9551,7 @@
       <c r="C107" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="D107" s="19">
+      <c r="D107" s="18">
         <v>43305</v>
       </c>
       <c r="F107" s="1" t="s">
@@ -9464,32 +9585,32 @@
       <c r="C109" s="4">
         <v>2011</v>
       </c>
-      <c r="D109" s="19">
+      <c r="D109" s="18">
         <v>43309</v>
       </c>
       <c r="F109" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="110" spans="1:7" s="40" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A110" s="39">
+    <row r="110" spans="1:7" s="39" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A110" s="38">
         <f t="shared" si="1"/>
         <v>108</v>
       </c>
-      <c r="B110" s="40" t="s">
+      <c r="B110" s="39" t="s">
         <v>221</v>
       </c>
-      <c r="C110" s="41">
+      <c r="C110" s="40">
         <v>1995</v>
       </c>
-      <c r="D110" s="19">
+      <c r="D110" s="18">
         <v>43310</v>
       </c>
-      <c r="E110" s="42"/>
-      <c r="F110" s="39" t="s">
+      <c r="E110" s="41"/>
+      <c r="F110" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="G110" s="43" t="s">
+      <c r="G110" s="42" t="s">
         <v>1127</v>
       </c>
     </row>
@@ -9504,7 +9625,7 @@
       <c r="C111" s="4" t="s">
         <v>1047</v>
       </c>
-      <c r="D111" s="19">
+      <c r="D111" s="18">
         <v>43319</v>
       </c>
       <c r="F111" s="1" t="s">
@@ -9522,7 +9643,7 @@
       <c r="C112" s="4" t="s">
         <v>1048</v>
       </c>
-      <c r="D112" s="19">
+      <c r="D112" s="18">
         <v>43327</v>
       </c>
       <c r="F112" s="1" t="s">
@@ -9543,7 +9664,7 @@
       <c r="C113" s="4" t="s">
         <v>1100</v>
       </c>
-      <c r="D113" s="19">
+      <c r="D113" s="18">
         <v>43346</v>
       </c>
       <c r="F113" s="1" t="s">
@@ -9561,10 +9682,10 @@
       <c r="C114" s="4" t="s">
         <v>1101</v>
       </c>
-      <c r="D114" s="19">
+      <c r="D114" s="18">
         <v>43353</v>
       </c>
-      <c r="E114" s="17" t="s">
+      <c r="E114" s="16" t="s">
         <v>226</v>
       </c>
       <c r="F114" s="1" t="s">
@@ -9585,7 +9706,7 @@
       <c r="C115" s="4" t="s">
         <v>1088</v>
       </c>
-      <c r="D115" s="19">
+      <c r="D115" s="18">
         <v>43373</v>
       </c>
       <c r="F115" s="1" t="s">
@@ -9603,7 +9724,7 @@
       <c r="C116" s="4" t="s">
         <v>1089</v>
       </c>
-      <c r="D116" s="19">
+      <c r="D116" s="18">
         <v>43375</v>
       </c>
       <c r="F116" s="1" t="s">
@@ -9615,16 +9736,16 @@
         <f>'2_watched_movies'!A116+1</f>
         <v>115</v>
       </c>
-      <c r="B117" s="24" t="s">
+      <c r="B117" s="23" t="s">
         <v>229</v>
       </c>
       <c r="C117" s="4">
         <v>2016</v>
       </c>
-      <c r="D117" s="19">
+      <c r="D117" s="18">
         <v>43387</v>
       </c>
-      <c r="E117" s="17" t="s">
+      <c r="E117" s="16" t="s">
         <v>230</v>
       </c>
       <c r="F117" s="1" t="s">
@@ -9645,7 +9766,7 @@
       <c r="C118" s="4">
         <v>1999</v>
       </c>
-      <c r="D118" s="19">
+      <c r="D118" s="18">
         <v>43389</v>
       </c>
       <c r="F118" s="1" t="s">
@@ -9663,7 +9784,7 @@
       <c r="C119" s="4">
         <v>2018</v>
       </c>
-      <c r="D119" s="19">
+      <c r="D119" s="18">
         <v>43416</v>
       </c>
       <c r="F119" s="1" t="s">
@@ -9681,7 +9802,7 @@
       <c r="C120" s="4">
         <v>2018</v>
       </c>
-      <c r="D120" s="19">
+      <c r="D120" s="18">
         <v>43438</v>
       </c>
       <c r="F120" s="1" t="s">
@@ -9699,10 +9820,10 @@
       <c r="C121" s="4">
         <v>2018</v>
       </c>
-      <c r="D121" s="19">
+      <c r="D121" s="18">
         <v>43450</v>
       </c>
-      <c r="E121" s="17" t="s">
+      <c r="E121" s="16" t="s">
         <v>235</v>
       </c>
       <c r="F121" s="1" t="s">
@@ -9717,13 +9838,13 @@
         <f t="shared" si="2"/>
         <v>120</v>
       </c>
-      <c r="B122" s="24" t="s">
+      <c r="B122" s="23" t="s">
         <v>237</v>
       </c>
       <c r="C122" s="4">
         <v>2001</v>
       </c>
-      <c r="D122" s="19">
+      <c r="D122" s="18">
         <v>43461</v>
       </c>
       <c r="F122" s="1" t="s">
@@ -9744,7 +9865,7 @@
       <c r="C123" s="4">
         <v>2004</v>
       </c>
-      <c r="D123" s="19">
+      <c r="D123" s="18">
         <v>43468</v>
       </c>
       <c r="F123" s="1" t="s">
@@ -9762,7 +9883,7 @@
       <c r="C124" s="4" t="s">
         <v>1090</v>
       </c>
-      <c r="D124" s="19">
+      <c r="D124" s="18">
         <v>43470</v>
       </c>
       <c r="F124" s="1" t="s">
@@ -9780,7 +9901,7 @@
       <c r="C125" s="4" t="s">
         <v>1091</v>
       </c>
-      <c r="D125" s="19">
+      <c r="D125" s="18">
         <v>43513</v>
       </c>
       <c r="F125" s="1" t="s">
@@ -9798,7 +9919,7 @@
       <c r="C126" s="4">
         <v>2016</v>
       </c>
-      <c r="D126" s="19">
+      <c r="D126" s="18">
         <v>43528</v>
       </c>
       <c r="F126" s="1" t="s">
@@ -9819,7 +9940,7 @@
       <c r="C127" s="4" t="s">
         <v>1091</v>
       </c>
-      <c r="D127" s="19">
+      <c r="D127" s="18">
         <v>43582</v>
       </c>
       <c r="F127" s="1" t="s">
@@ -9837,7 +9958,7 @@
       <c r="C128" s="4" t="s">
         <v>1092</v>
       </c>
-      <c r="D128" s="19">
+      <c r="D128" s="18">
         <v>43590</v>
       </c>
       <c r="F128" s="1" t="s">
@@ -9855,7 +9976,7 @@
       <c r="C129" s="4" t="s">
         <v>1091</v>
       </c>
-      <c r="D129" s="19">
+      <c r="D129" s="18">
         <v>43617</v>
       </c>
       <c r="F129" s="1" t="s">
@@ -9891,7 +10012,7 @@
       <c r="C131" s="4">
         <v>2019</v>
       </c>
-      <c r="D131" s="19">
+      <c r="D131" s="18">
         <v>43708</v>
       </c>
       <c r="F131" s="1" t="s">
@@ -10148,11 +10269,11 @@
         <f>'2_watched_movies'!A149+1</f>
         <v>148</v>
       </c>
-      <c r="B150" s="24" t="s">
+      <c r="B150" s="23" t="s">
         <v>1074</v>
       </c>
-      <c r="C150" s="23"/>
-      <c r="D150" s="20"/>
+      <c r="C150" s="22"/>
+      <c r="D150" s="19"/>
       <c r="F150" s="1" t="s">
         <v>248</v>
       </c>
@@ -10212,7 +10333,7 @@
         <v>248</v>
       </c>
       <c r="G154" s="12" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="155" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -10266,11 +10387,14 @@
         <v>273</v>
       </c>
       <c r="C158" s="4"/>
-      <c r="D158" s="29" t="s">
+      <c r="D158" s="28" t="s">
         <v>274</v>
       </c>
       <c r="F158" s="1" t="s">
         <v>248</v>
+      </c>
+      <c r="G158" s="1" t="s">
+        <v>1281</v>
       </c>
     </row>
     <row r="159" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -10661,7 +10785,7 @@
         <v>305</v>
       </c>
       <c r="C188" s="4"/>
-      <c r="E188" s="17" t="s">
+      <c r="E188" s="16" t="s">
         <v>306</v>
       </c>
       <c r="F188" s="1" t="s">
@@ -10679,10 +10803,10 @@
       <c r="C189" s="4" t="s">
         <v>1134</v>
       </c>
-      <c r="D189" s="19">
+      <c r="D189" s="18">
         <v>42797</v>
       </c>
-      <c r="E189" s="17" t="s">
+      <c r="E189" s="16" t="s">
         <v>171</v>
       </c>
       <c r="F189" s="1" t="s">
@@ -10869,10 +10993,10 @@
       <c r="C203" s="4" t="s">
         <v>1135</v>
       </c>
-      <c r="D203" s="19">
+      <c r="D203" s="18">
         <v>42925</v>
       </c>
-      <c r="E203" s="17" t="s">
+      <c r="E203" s="16" t="s">
         <v>110</v>
       </c>
       <c r="F203" s="1" t="s">
@@ -10968,7 +11092,7 @@
         <v>345</v>
       </c>
       <c r="C209" s="4"/>
-      <c r="D209" s="19">
+      <c r="D209" s="18">
         <v>43071</v>
       </c>
       <c r="F209" s="1" t="s">
@@ -11235,11 +11359,11 @@
         <f>'2_watched_movies'!A227+1</f>
         <v>226</v>
       </c>
-      <c r="B228" s="30" t="s">
+      <c r="B228" s="29" t="s">
         <v>380</v>
       </c>
-      <c r="C228" s="23"/>
-      <c r="D228" s="20"/>
+      <c r="C228" s="22"/>
+      <c r="D228" s="19"/>
       <c r="F228" s="1" t="s">
         <v>370</v>
       </c>
@@ -11336,7 +11460,7 @@
       <c r="C235" s="4">
         <v>2021</v>
       </c>
-      <c r="D235" s="19">
+      <c r="D235" s="18">
         <v>44303</v>
       </c>
     </row>
@@ -11351,10 +11475,10 @@
       <c r="C236" s="4">
         <v>2021</v>
       </c>
-      <c r="D236" s="19">
+      <c r="D236" s="18">
         <v>44332</v>
       </c>
-      <c r="E236" s="17" t="s">
+      <c r="E236" s="16" t="s">
         <v>391</v>
       </c>
     </row>
@@ -11369,10 +11493,10 @@
       <c r="C237" s="4">
         <v>2011</v>
       </c>
-      <c r="D237" s="19">
+      <c r="D237" s="18">
         <v>44340</v>
       </c>
-      <c r="E237" s="17" t="s">
+      <c r="E237" s="16" t="s">
         <v>393</v>
       </c>
       <c r="G237" s="1" t="s">
@@ -11388,10 +11512,10 @@
         <v>395</v>
       </c>
       <c r="C238" s="4"/>
-      <c r="D238" s="19">
+      <c r="D238" s="18">
         <v>44343</v>
       </c>
-      <c r="E238" s="17" t="s">
+      <c r="E238" s="16" t="s">
         <v>396</v>
       </c>
       <c r="G238" s="1" t="s">
@@ -11409,7 +11533,7 @@
       <c r="C239" s="4">
         <v>1986</v>
       </c>
-      <c r="D239" s="19">
+      <c r="D239" s="18">
         <v>44351</v>
       </c>
     </row>
@@ -11418,13 +11542,13 @@
         <f>'2_watched_movies'!A239+1</f>
         <v>238</v>
       </c>
-      <c r="B240" s="24" t="s">
-        <v>1211</v>
-      </c>
-      <c r="C240" s="23">
+      <c r="B240" s="23" t="s">
+        <v>1209</v>
+      </c>
+      <c r="C240" s="22">
         <v>1997</v>
       </c>
-      <c r="D240" s="19">
+      <c r="D240" s="18">
         <v>44346</v>
       </c>
       <c r="F240" s="1" t="s">
@@ -11440,7 +11564,7 @@
         <v>400</v>
       </c>
       <c r="C241" s="4"/>
-      <c r="D241" s="19">
+      <c r="D241" s="18">
         <v>44380</v>
       </c>
       <c r="F241" s="1" t="s">
@@ -11459,10 +11583,10 @@
         <v>402</v>
       </c>
       <c r="C242" s="4"/>
-      <c r="D242" s="19">
+      <c r="D242" s="18">
         <v>44380</v>
       </c>
-      <c r="E242" s="17" t="s">
+      <c r="E242" s="16" t="s">
         <v>403</v>
       </c>
       <c r="F242" s="1" t="s">
@@ -11483,7 +11607,7 @@
       <c r="C243" s="4">
         <v>2021</v>
       </c>
-      <c r="D243" s="19">
+      <c r="D243" s="18">
         <v>44401</v>
       </c>
       <c r="G243" s="1" t="s">
@@ -11505,11 +11629,11 @@
         <f t="shared" si="7"/>
         <v>243</v>
       </c>
-      <c r="B245" s="30" t="s">
+      <c r="B245" s="29" t="s">
         <v>1137</v>
       </c>
       <c r="C245" s="4"/>
-      <c r="D245" s="29" t="s">
+      <c r="D245" s="28" t="s">
         <v>1119</v>
       </c>
       <c r="G245" s="12" t="s">
@@ -11689,7 +11813,7 @@
         <v>1102</v>
       </c>
       <c r="C260" s="4"/>
-      <c r="D260" s="19">
+      <c r="D260" s="18">
         <v>44437</v>
       </c>
       <c r="G260" s="1" t="s">
@@ -11733,11 +11857,11 @@
         <f>'2_watched_movies'!A262+1</f>
         <v>261</v>
       </c>
-      <c r="B263" s="24" t="s">
+      <c r="B263" s="23" t="s">
         <v>430</v>
       </c>
-      <c r="C263" s="23"/>
-      <c r="D263" s="20"/>
+      <c r="C263" s="22"/>
+      <c r="D263" s="19"/>
     </row>
     <row r="264" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
@@ -11825,14 +11949,14 @@
         <f t="shared" si="8"/>
         <v>268</v>
       </c>
-      <c r="B270" s="30" t="s">
+      <c r="B270" s="29" t="s">
         <v>440</v>
       </c>
       <c r="C270" s="4"/>
-      <c r="D270" s="19">
+      <c r="D270" s="18">
         <v>44448</v>
       </c>
-      <c r="E270" s="17" t="s">
+      <c r="E270" s="16" t="s">
         <v>403</v>
       </c>
       <c r="F270" s="1" t="s">
@@ -11869,11 +11993,11 @@
         <f>'2_watched_movies'!A272+1</f>
         <v>271</v>
       </c>
-      <c r="B273" s="24" t="s">
-        <v>1210</v>
-      </c>
-      <c r="C273" s="23"/>
-      <c r="D273" s="20"/>
+      <c r="B273" s="23" t="s">
+        <v>1208</v>
+      </c>
+      <c r="C273" s="22"/>
+      <c r="D273" s="19"/>
     </row>
     <row r="274" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
@@ -11884,7 +12008,7 @@
         <v>444</v>
       </c>
       <c r="C274" s="4"/>
-      <c r="D274" s="19">
+      <c r="D274" s="18">
         <v>44550</v>
       </c>
     </row>
@@ -11979,7 +12103,7 @@
         <v>453</v>
       </c>
       <c r="C282" s="4"/>
-      <c r="D282" s="19">
+      <c r="D282" s="18">
         <v>44458</v>
       </c>
       <c r="G282" s="1" t="s">
@@ -11997,10 +12121,10 @@
       <c r="C283" s="4">
         <v>2019</v>
       </c>
-      <c r="D283" s="19">
+      <c r="D283" s="18">
         <v>44499</v>
       </c>
-      <c r="E283" s="17" t="s">
+      <c r="E283" s="16" t="s">
         <v>456</v>
       </c>
     </row>
@@ -12015,10 +12139,10 @@
       <c r="C284" s="4">
         <v>2021</v>
       </c>
-      <c r="D284" s="19">
+      <c r="D284" s="18">
         <v>44520</v>
       </c>
-      <c r="E284" s="17" t="s">
+      <c r="E284" s="16" t="s">
         <v>458</v>
       </c>
     </row>
@@ -12033,10 +12157,10 @@
       <c r="C285" s="4">
         <v>2013</v>
       </c>
-      <c r="D285" s="19">
+      <c r="D285" s="18">
         <v>44545</v>
       </c>
-      <c r="E285" s="17" t="s">
+      <c r="E285" s="16" t="s">
         <v>142</v>
       </c>
     </row>
@@ -12051,10 +12175,10 @@
       <c r="C286" s="4">
         <v>2021</v>
       </c>
-      <c r="D286" s="19">
+      <c r="D286" s="18">
         <v>44548</v>
       </c>
-      <c r="E286" s="17" t="s">
+      <c r="E286" s="16" t="s">
         <v>461</v>
       </c>
       <c r="G286" s="1" t="s">
@@ -12106,17 +12230,17 @@
     <row r="291" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A291" s="1"/>
       <c r="B291" s="8" t="s">
+        <v>1187</v>
+      </c>
+      <c r="C291" s="4"/>
+      <c r="D291" s="28" t="s">
         <v>1189</v>
       </c>
-      <c r="C291" s="4"/>
-      <c r="D291" s="29" t="s">
-        <v>1191</v>
-      </c>
-      <c r="E291" s="17" t="s">
-        <v>1192</v>
+      <c r="E291" s="16" t="s">
+        <v>1190</v>
       </c>
       <c r="G291" s="1" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="292" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -12125,12 +12249,12 @@
         <v>289</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
       <c r="C292" s="4">
         <v>2021</v>
       </c>
-      <c r="D292" s="29" t="s">
+      <c r="D292" s="28" t="s">
         <v>467</v>
       </c>
       <c r="G292" s="1" t="s">
@@ -12142,11 +12266,11 @@
         <f>'2_watched_movies'!A292+1</f>
         <v>290</v>
       </c>
-      <c r="B293" s="30" t="s">
+      <c r="B293" s="29" t="s">
         <v>469</v>
       </c>
-      <c r="C293" s="23"/>
-      <c r="D293" s="21" t="s">
+      <c r="C293" s="22"/>
+      <c r="D293" s="20" t="s">
         <v>1003</v>
       </c>
       <c r="G293" s="1" t="s">
@@ -12158,11 +12282,11 @@
         <f>A293+1</f>
         <v>291</v>
       </c>
-      <c r="B294" s="30" t="s">
-        <v>1203</v>
-      </c>
-      <c r="C294" s="23"/>
-      <c r="D294" s="20"/>
+      <c r="B294" s="29" t="s">
+        <v>1201</v>
+      </c>
+      <c r="C294" s="22"/>
+      <c r="D294" s="19"/>
     </row>
     <row r="295" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A295" s="1">
@@ -12170,12 +12294,12 @@
         <v>292</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>1204</v>
+        <v>1202</v>
       </c>
       <c r="C295" s="4">
         <v>2022</v>
       </c>
-      <c r="D295" s="29" t="s">
+      <c r="D295" s="28" t="s">
         <v>471</v>
       </c>
       <c r="G295" s="1" t="s">
@@ -12191,10 +12315,10 @@
         <v>473</v>
       </c>
       <c r="C296" s="4"/>
-      <c r="D296" s="29" t="s">
+      <c r="D296" s="28" t="s">
         <v>474</v>
       </c>
-      <c r="E296" s="23">
+      <c r="E296" s="22">
         <v>7</v>
       </c>
       <c r="G296" s="1" t="s">
@@ -12206,13 +12330,13 @@
         <f>'2_watched_movies'!A296+1</f>
         <v>294</v>
       </c>
-      <c r="B297" s="24" t="s">
+      <c r="B297" s="23" t="s">
         <v>476</v>
       </c>
       <c r="C297" s="4">
         <v>2021</v>
       </c>
-      <c r="D297" s="21" t="s">
+      <c r="D297" s="20" t="s">
         <v>477</v>
       </c>
       <c r="G297" s="1" t="s">
@@ -12234,13 +12358,13 @@
         <f>'2_watched_movies'!A298+1</f>
         <v>296</v>
       </c>
-      <c r="B299" s="24" t="s">
+      <c r="B299" s="23" t="s">
         <v>476</v>
       </c>
       <c r="C299" s="4">
         <v>2021</v>
       </c>
-      <c r="D299" s="21" t="s">
+      <c r="D299" s="20" t="s">
         <v>999</v>
       </c>
       <c r="G299" s="1" t="s">
@@ -12258,10 +12382,10 @@
       <c r="C300" s="4">
         <v>2014</v>
       </c>
-      <c r="D300" s="29" t="s">
+      <c r="D300" s="28" t="s">
         <v>480</v>
       </c>
-      <c r="E300" s="17">
+      <c r="E300" s="16">
         <v>6</v>
       </c>
     </row>
@@ -12276,10 +12400,10 @@
       <c r="C301" s="4">
         <v>2022</v>
       </c>
-      <c r="D301" s="29" t="s">
+      <c r="D301" s="28" t="s">
         <v>482</v>
       </c>
-      <c r="E301" s="17">
+      <c r="E301" s="16">
         <v>7.3</v>
       </c>
     </row>
@@ -12289,12 +12413,12 @@
         <v>298</v>
       </c>
       <c r="B302" s="1" t="s">
-        <v>1206</v>
+        <v>1204</v>
       </c>
       <c r="C302" s="4">
         <v>2022</v>
       </c>
-      <c r="D302" s="29" t="s">
+      <c r="D302" s="28" t="s">
         <v>483</v>
       </c>
     </row>
@@ -12306,10 +12430,10 @@
         <v>484</v>
       </c>
       <c r="C303" s="4"/>
-      <c r="D303" s="29" t="s">
+      <c r="D303" s="28" t="s">
         <v>485</v>
       </c>
-      <c r="E303" s="17">
+      <c r="E303" s="16">
         <v>7.8</v>
       </c>
     </row>
@@ -12323,10 +12447,10 @@
       <c r="C304" s="4">
         <v>2017</v>
       </c>
-      <c r="D304" s="29" t="s">
+      <c r="D304" s="28" t="s">
         <v>485</v>
       </c>
-      <c r="E304" s="17">
+      <c r="E304" s="16">
         <v>6.5</v>
       </c>
       <c r="G304" s="1" t="s">
@@ -12338,15 +12462,15 @@
         <v>301</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>1209</v>
+        <v>1207</v>
       </c>
       <c r="C305" s="4">
         <v>2022</v>
       </c>
-      <c r="D305" s="29" t="s">
+      <c r="D305" s="28" t="s">
         <v>486</v>
       </c>
-      <c r="E305" s="17">
+      <c r="E305" s="16">
         <v>7</v>
       </c>
       <c r="G305" s="1" t="s">
@@ -12363,10 +12487,10 @@
       <c r="C306" s="4">
         <v>2019</v>
       </c>
-      <c r="D306" s="29">
+      <c r="D306" s="28">
         <v>2019</v>
       </c>
-      <c r="E306" s="17">
+      <c r="E306" s="16">
         <v>7.8</v>
       </c>
       <c r="G306" s="1" t="s">
@@ -12378,15 +12502,15 @@
         <v>303</v>
       </c>
       <c r="B307" s="1" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="C307" s="4">
         <v>2001</v>
       </c>
-      <c r="D307" s="28" t="s">
+      <c r="D307" s="27" t="s">
         <v>981</v>
       </c>
-      <c r="E307" s="16">
+      <c r="E307" s="15">
         <v>6.8</v>
       </c>
       <c r="G307" t="s">
@@ -12398,15 +12522,15 @@
         <v>304</v>
       </c>
       <c r="B308" s="1" t="s">
-        <v>1207</v>
+        <v>1205</v>
       </c>
       <c r="C308" s="4">
         <v>2022</v>
       </c>
-      <c r="D308" s="29" t="s">
+      <c r="D308" s="28" t="s">
         <v>1043</v>
       </c>
-      <c r="E308" s="16">
+      <c r="E308" s="15">
         <v>7.6</v>
       </c>
     </row>
@@ -12414,16 +12538,16 @@
       <c r="A309" s="1">
         <v>305</v>
       </c>
-      <c r="B309" s="30" t="s">
-        <v>1202</v>
+      <c r="B309" s="29" t="s">
+        <v>1200</v>
       </c>
       <c r="C309" s="4">
         <v>2023</v>
       </c>
-      <c r="D309" s="20" t="s">
+      <c r="D309" s="19" t="s">
         <v>983</v>
       </c>
-      <c r="E309" s="16">
+      <c r="E309" s="15">
         <v>8</v>
       </c>
     </row>
@@ -12431,11 +12555,11 @@
       <c r="A310" s="1">
         <v>306</v>
       </c>
-      <c r="B310" s="30" t="s">
+      <c r="B310" s="29" t="s">
         <v>1001</v>
       </c>
-      <c r="C310" s="28"/>
-      <c r="D310" s="21">
+      <c r="C310" s="27"/>
+      <c r="D310" s="20">
         <v>2023</v>
       </c>
     </row>
@@ -12443,11 +12567,11 @@
       <c r="A311">
         <v>307</v>
       </c>
-      <c r="B311" s="24" t="s">
+      <c r="B311" s="23" t="s">
         <v>1066</v>
       </c>
-      <c r="C311" s="28"/>
-      <c r="D311" s="21" t="s">
+      <c r="C311" s="27"/>
+      <c r="D311" s="20" t="s">
         <v>1015</v>
       </c>
       <c r="G311" s="1" t="s">
@@ -12458,14 +12582,14 @@
       <c r="A312" s="1">
         <v>308</v>
       </c>
-      <c r="B312" s="24" t="s">
-        <v>1205</v>
-      </c>
-      <c r="C312" s="28"/>
-      <c r="D312" s="21" t="s">
+      <c r="B312" s="23" t="s">
+        <v>1203</v>
+      </c>
+      <c r="C312" s="27"/>
+      <c r="D312" s="20" t="s">
         <v>1021</v>
       </c>
-      <c r="E312" s="18" t="s">
+      <c r="E312" s="17" t="s">
         <v>1023</v>
       </c>
       <c r="G312" s="6" t="s">
@@ -12476,16 +12600,16 @@
       <c r="A313" s="1">
         <v>309</v>
       </c>
-      <c r="B313" s="25" t="s">
+      <c r="B313" s="24" t="s">
         <v>1067</v>
       </c>
-      <c r="C313" s="28">
+      <c r="C313" s="27">
         <v>2021</v>
       </c>
-      <c r="D313" s="21" t="s">
+      <c r="D313" s="20" t="s">
         <v>1024</v>
       </c>
-      <c r="E313" s="17" t="s">
+      <c r="E313" s="16" t="s">
         <v>1025</v>
       </c>
       <c r="G313" s="12" t="s">
@@ -12496,14 +12620,14 @@
       <c r="A314" s="1">
         <v>310</v>
       </c>
-      <c r="B314" s="30" t="s">
+      <c r="B314" s="29" t="s">
         <v>1032</v>
       </c>
-      <c r="C314" s="28"/>
-      <c r="D314" s="21" t="s">
+      <c r="C314" s="27"/>
+      <c r="D314" s="20" t="s">
         <v>1031</v>
       </c>
-      <c r="E314" s="17" t="s">
+      <c r="E314" s="16" t="s">
         <v>1033</v>
       </c>
     </row>
@@ -12511,14 +12635,14 @@
       <c r="A315">
         <v>311</v>
       </c>
-      <c r="B315" s="24" t="s">
+      <c r="B315" s="23" t="s">
         <v>1068</v>
       </c>
-      <c r="C315" s="28"/>
-      <c r="D315" s="21" t="s">
+      <c r="C315" s="27"/>
+      <c r="D315" s="20" t="s">
         <v>1042</v>
       </c>
-      <c r="E315" s="16">
+      <c r="E315" s="15">
         <v>5</v>
       </c>
       <c r="G315" s="12" t="s">
@@ -12529,14 +12653,14 @@
       <c r="A316" s="1">
         <v>312</v>
       </c>
-      <c r="B316" s="24" t="s">
+      <c r="B316" s="23" t="s">
         <v>1055</v>
       </c>
-      <c r="C316" s="28"/>
-      <c r="D316" s="21" t="s">
+      <c r="C316" s="27"/>
+      <c r="D316" s="20" t="s">
         <v>1056</v>
       </c>
-      <c r="E316" s="16">
+      <c r="E316" s="15">
         <v>7</v>
       </c>
     </row>
@@ -12544,11 +12668,11 @@
       <c r="A317" s="1">
         <v>313</v>
       </c>
-      <c r="B317" s="26" t="s">
+      <c r="B317" s="25" t="s">
         <v>1052</v>
       </c>
-      <c r="C317" s="28"/>
-      <c r="D317" s="21" t="s">
+      <c r="C317" s="27"/>
+      <c r="D317" s="20" t="s">
         <v>1059</v>
       </c>
     </row>
@@ -12556,52 +12680,52 @@
       <c r="A318" s="1">
         <v>314</v>
       </c>
-      <c r="B318" s="25" t="s">
+      <c r="B318" s="24" t="s">
         <v>1069</v>
       </c>
-      <c r="C318" s="28">
+      <c r="C318" s="27">
         <v>2021</v>
       </c>
-      <c r="D318" s="21" t="s">
+      <c r="D318" s="20" t="s">
         <v>1064</v>
       </c>
-      <c r="E318" s="18" t="s">
+      <c r="E318" s="17" t="s">
         <v>1065</v>
       </c>
       <c r="G318" s="12" t="s">
         <v>1063</v>
       </c>
     </row>
-    <row r="319" spans="1:7" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A319" s="33">
+    <row r="319" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A319" s="32">
         <v>315</v>
       </c>
-      <c r="B319" s="33" t="s">
+      <c r="B319" s="32" t="s">
         <v>1114</v>
       </c>
-      <c r="C319" s="34">
+      <c r="C319" s="33">
         <v>2001</v>
       </c>
-      <c r="D319" s="34" t="s">
+      <c r="D319" s="33" t="s">
         <v>1116</v>
       </c>
-      <c r="E319" s="35" t="s">
+      <c r="E319" s="34" t="s">
         <v>1115</v>
       </c>
-      <c r="G319" s="36"/>
+      <c r="G319" s="35"/>
     </row>
     <row r="320" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A320" s="1">
         <v>316</v>
       </c>
-      <c r="B320" s="25" t="s">
+      <c r="B320" s="24" t="s">
         <v>1110</v>
       </c>
       <c r="C320" s="4"/>
-      <c r="D320" s="29" t="s">
+      <c r="D320" s="28" t="s">
         <v>1111</v>
       </c>
-      <c r="E320" s="18" t="s">
+      <c r="E320" s="17" t="s">
         <v>1112</v>
       </c>
     </row>
@@ -12609,83 +12733,77 @@
       <c r="A321" s="1">
         <v>317</v>
       </c>
-      <c r="B321" s="25" t="s">
+      <c r="B321" s="24" t="s">
         <v>1120</v>
       </c>
       <c r="C321" s="4"/>
-      <c r="D321" s="29" t="s">
+      <c r="D321" s="28" t="s">
         <v>1111</v>
       </c>
-      <c r="E321" s="18" t="s">
+      <c r="E321" s="17" t="s">
         <v>1065</v>
       </c>
       <c r="G321" s="12" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="322" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A322" s="1">
         <v>318</v>
       </c>
-      <c r="B322" s="24" t="s">
-        <v>1180</v>
+      <c r="B322" s="23" t="s">
+        <v>1179</v>
       </c>
       <c r="C322" s="4">
         <v>1988</v>
       </c>
-      <c r="D322" s="29" t="s">
+      <c r="D322" s="28" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G322" s="6" t="s">
         <v>1181</v>
-      </c>
-      <c r="G322" s="6" t="s">
-        <v>1182</v>
       </c>
     </row>
     <row r="323" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A323" s="1">
         <v>319</v>
       </c>
-      <c r="B323" s="24" t="s">
+      <c r="B323" s="23" t="s">
         <v>1158</v>
       </c>
       <c r="C323" s="4"/>
-      <c r="D323" s="29" t="s">
-        <v>1194</v>
-      </c>
-      <c r="E323" s="18" t="s">
+      <c r="D323" s="28" t="s">
+        <v>1192</v>
+      </c>
+      <c r="E323" s="17" t="s">
         <v>1112</v>
       </c>
       <c r="G323" s="1" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="324" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A324" s="1">
-        <v>320</v>
-      </c>
-      <c r="B324" s="25" t="s">
-        <v>1201</v>
+      <c r="A324" s="1"/>
+      <c r="B324" s="23" t="s">
+        <v>1269</v>
       </c>
       <c r="C324" s="4"/>
-      <c r="E324" s="48" t="s">
-        <v>1200</v>
-      </c>
+      <c r="D324" s="28"/>
+      <c r="E324" s="17"/>
       <c r="G324" s="1" t="s">
-        <v>1198</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="325" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A325" s="1">
-        <v>321</v>
-      </c>
-      <c r="B325" s="25" t="s">
-        <v>1197</v>
+        <v>320</v>
+      </c>
+      <c r="B325" s="24" t="s">
+        <v>1199</v>
       </c>
       <c r="C325" s="4"/>
-      <c r="D325" s="29" t="s">
-        <v>1199</v>
-      </c>
-      <c r="E325" s="48" t="s">
-        <v>1200</v>
+      <c r="E325" s="47" t="s">
+        <v>1198</v>
       </c>
       <c r="G325" s="1" t="s">
         <v>1196</v>
@@ -12693,107 +12811,161 @@
     </row>
     <row r="326" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A326" s="1">
+        <v>321</v>
+      </c>
+      <c r="B326" s="24" t="s">
+        <v>1195</v>
+      </c>
+      <c r="C326" s="4"/>
+      <c r="D326" s="28" t="s">
+        <v>1197</v>
+      </c>
+      <c r="E326" s="47" t="s">
+        <v>1198</v>
+      </c>
+      <c r="G326" s="1" t="s">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="327" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A327" s="1">
         <v>322</v>
       </c>
-      <c r="B326" s="25" t="s">
-        <v>1219</v>
-      </c>
-      <c r="C326" s="4"/>
-      <c r="D326" s="29" t="s">
+      <c r="B327" s="24" t="s">
         <v>1217</v>
       </c>
-      <c r="E326" s="48" t="s">
-        <v>1248</v>
-      </c>
-      <c r="G326" s="1" t="s">
-        <v>1218</v>
-      </c>
-    </row>
-    <row r="327" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A327" s="1">
-        <v>323</v>
-      </c>
-      <c r="B327" s="25" t="s">
-        <v>1221</v>
-      </c>
-      <c r="D327" s="29" t="s">
+      <c r="C327" s="4"/>
+      <c r="D327" s="28" t="s">
+        <v>1215</v>
+      </c>
+      <c r="E327" s="47" t="s">
+        <v>1243</v>
+      </c>
+      <c r="G327" s="1" t="s">
         <v>1216</v>
-      </c>
-      <c r="E327" s="48" t="s">
-        <v>1222</v>
-      </c>
-      <c r="G327" s="1" t="s">
-        <v>1220</v>
       </c>
     </row>
     <row r="328" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A328" s="1">
+        <v>323</v>
+      </c>
+      <c r="B328" s="24" t="s">
+        <v>1219</v>
+      </c>
+      <c r="D328" s="28" t="s">
+        <v>1214</v>
+      </c>
+      <c r="E328" s="47" t="s">
+        <v>1220</v>
+      </c>
+      <c r="G328" s="1" t="s">
+        <v>1218</v>
+      </c>
+    </row>
+    <row r="329" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A329" s="1">
         <v>324</v>
       </c>
-      <c r="B328" s="52" t="s">
-        <v>1243</v>
-      </c>
-      <c r="C328" s="4">
+      <c r="B329" s="51" t="s">
+        <v>1238</v>
+      </c>
+      <c r="C329" s="4">
         <v>2015</v>
       </c>
-      <c r="D328" s="29" t="s">
-        <v>1244</v>
-      </c>
-      <c r="E328" s="48" t="s">
+      <c r="D329" s="28" t="s">
+        <v>1239</v>
+      </c>
+      <c r="E329" s="47" t="s">
         <v>1065</v>
-      </c>
-    </row>
-    <row r="329" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A329" s="1">
-        <v>325</v>
-      </c>
-      <c r="B329" s="25" t="s">
-        <v>1247</v>
-      </c>
-      <c r="C329" s="4">
-        <v>2000</v>
-      </c>
-      <c r="D329" s="29" t="s">
-        <v>1245</v>
-      </c>
-      <c r="E329" s="48" t="s">
-        <v>1112</v>
-      </c>
-      <c r="G329" s="1" t="s">
-        <v>1246</v>
       </c>
     </row>
     <row r="330" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A330" s="1">
+        <v>325</v>
+      </c>
+      <c r="B330" s="24" t="s">
+        <v>1242</v>
+      </c>
+      <c r="C330" s="4">
+        <v>2000</v>
+      </c>
+      <c r="D330" s="28" t="s">
+        <v>1240</v>
+      </c>
+      <c r="E330" s="47" t="s">
+        <v>1112</v>
+      </c>
+      <c r="G330" s="1" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="331" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A331" s="1">
         <v>326</v>
       </c>
-      <c r="B330" s="25" t="s">
+      <c r="B331" s="24" t="s">
+        <v>1266</v>
+      </c>
+      <c r="C331" s="4">
+        <v>2023</v>
+      </c>
+      <c r="D331" s="28" t="s">
+        <v>1265</v>
+      </c>
+      <c r="E331" s="47" t="s">
+        <v>1264</v>
+      </c>
+      <c r="G331" s="21" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="332" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A332" s="1">
+        <v>327</v>
+      </c>
+      <c r="B332" s="24" t="s">
+        <v>1268</v>
+      </c>
+      <c r="C332" s="4">
+        <v>1995</v>
+      </c>
+      <c r="D332" s="28" t="s">
+        <v>1267</v>
+      </c>
+    </row>
+    <row r="333" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A333" s="1">
+        <v>328</v>
+      </c>
+      <c r="B333" s="24" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C333" s="4">
+        <v>2014</v>
+      </c>
+      <c r="D333" s="28" t="s">
         <v>1272</v>
       </c>
-      <c r="C330" s="4">
-        <v>2023</v>
-      </c>
-      <c r="D330" s="29" t="s">
-        <v>1271</v>
-      </c>
-      <c r="E330" s="48" t="s">
-        <v>1270</v>
-      </c>
-      <c r="G330" s="22" t="s">
-        <v>1269</v>
-      </c>
-    </row>
-    <row r="331" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C331" s="4"/>
-    </row>
-    <row r="332" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C332" s="4"/>
-    </row>
-    <row r="333" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C333" s="4"/>
-    </row>
-    <row r="334" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C334" s="4"/>
+      <c r="E333" s="47" t="s">
+        <v>1273</v>
+      </c>
+    </row>
+    <row r="334" spans="1:7" s="32" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A334" s="32">
+        <v>329</v>
+      </c>
+      <c r="B334" s="32" t="s">
+        <v>1285</v>
+      </c>
+      <c r="C334" s="45">
+        <v>2024</v>
+      </c>
+      <c r="D334" s="33" t="s">
+        <v>1286</v>
+      </c>
+      <c r="E334" s="46" t="s">
+        <v>1287</v>
+      </c>
     </row>
     <row r="335" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C335" s="4"/>
@@ -14813,6 +14985,9 @@
     </row>
     <row r="1007" spans="3:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1007" s="4"/>
+    </row>
+    <row r="1008" spans="3:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1008" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5"/>
@@ -14825,7 +15000,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H1008"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
@@ -14845,10 +15020,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1262</v>
+        <v>1256</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1250</v>
+        <v>1244</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1051</v>
@@ -14873,18 +15048,18 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:6" s="40" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="39">
+    <row r="3" spans="1:6" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="38">
         <v>2</v>
       </c>
-      <c r="B3" s="43" t="s">
-        <v>1161</v>
-      </c>
-      <c r="C3" s="39" t="s">
+      <c r="B3" s="42" t="s">
+        <v>1160</v>
+      </c>
+      <c r="C3" s="38" t="s">
         <v>587</v>
       </c>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -15004,7 +15179,7 @@
         <v>598</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1261</v>
+        <v>1255</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -15056,7 +15231,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>1267</v>
+        <v>1261</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>1038</v>
@@ -15339,13 +15514,13 @@
         <v>13</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>1251</v>
+        <v>1245</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>511</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>1252</v>
+        <v>1246</v>
       </c>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
@@ -15423,86 +15598,86 @@
       </c>
     </row>
     <row r="48" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="14" t="s">
+      <c r="B48" s="13" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="13" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="31" t="s">
         <v>1162</v>
       </c>
     </row>
-    <row r="49" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="14" t="s">
-        <v>1113</v>
-      </c>
-    </row>
-    <row r="50" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="32" t="s">
+    <row r="51" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="31" t="s">
         <v>1163</v>
       </c>
-    </row>
-    <row r="51" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="32" t="s">
+      <c r="E51" s="1" t="s">
         <v>1164</v>
       </c>
-      <c r="E51" s="1" t="s">
-        <v>1165</v>
-      </c>
     </row>
     <row r="52" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="32" t="s">
+      <c r="B52" s="31" t="s">
+        <v>1173</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>1247</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>1248</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="31" t="s">
         <v>1174</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="E53" s="1" t="s">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="31" t="s">
+        <v>1249</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>1250</v>
+      </c>
+      <c r="E54" s="1"/>
+    </row>
+    <row r="55" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="31" t="s">
         <v>1253</v>
       </c>
-      <c r="F52" s="1" t="s">
+      <c r="C55" s="1" t="s">
         <v>1254</v>
       </c>
-    </row>
-    <row r="53" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="32" t="s">
-        <v>1175</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>1178</v>
-      </c>
-    </row>
-    <row r="54" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="32" t="s">
-        <v>1255</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>1256</v>
-      </c>
-      <c r="E54" s="1"/>
-    </row>
-    <row r="55" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="32" t="s">
-        <v>1259</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>1260</v>
-      </c>
       <c r="E55" s="1"/>
     </row>
     <row r="56" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="32" t="s">
-        <v>1257</v>
+      <c r="B56" s="31" t="s">
+        <v>1251</v>
       </c>
       <c r="C56" s="1"/>
       <c r="E56" s="1" t="s">
-        <v>1258</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="57" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E57" s="1"/>
     </row>
     <row r="58" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="32"/>
+      <c r="B58" s="31"/>
       <c r="C58" s="1"/>
       <c r="E58" s="1"/>
     </row>
     <row r="59" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="60" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="8" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="61" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -15517,8 +15692,8 @@
     <row r="66" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="67" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="68" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="44" t="s">
-        <v>1177</v>
+      <c r="B68" s="43" t="s">
+        <v>1176</v>
       </c>
     </row>
     <row r="69" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -15528,12 +15703,12 @@
     <row r="73" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="74" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="8" t="s">
-        <v>1263</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="75" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="32" t="s">
-        <v>1264</v>
+      <c r="B75" s="31" t="s">
+        <v>1258</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>1030</v>
@@ -15541,15 +15716,15 @@
     </row>
     <row r="76" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="1" t="s">
-        <v>1265</v>
+        <v>1259</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1266</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="77" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="1" t="s">
-        <v>1268</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="78" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -16506,12 +16681,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
     </row>
   </sheetData>
@@ -16595,7 +16770,7 @@
         <v>496</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1193</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -18137,37 +18312,37 @@
     <row r="53" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="54" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="8" t="s">
-        <v>1236</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="8" t="s">
-        <v>1240</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
-        <v>1237</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">
-        <v>1238</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
-        <v>1239</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
-        <v>1241</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="s">
-        <v>1242</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated movie and book list
</commit_message>
<xml_diff>
--- a/thongnd_everything_list.xlsx
+++ b/thongnd_everything_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\ドキュメント\GitHub\My_Everything_Lists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52578B1C-D122-4515-B953-753FCDC2E1E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA666C69-986A-4BC5-8547-67D955FA4577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1_todolist" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1891" uniqueCount="1291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1902" uniqueCount="1302">
   <si>
     <t>ID</t>
   </si>
@@ -4225,10 +4225,6 @@
   </si>
   <si>
     <t>Anaconda</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>Phim mãng xà ăn thịt người, trước thường được chiếu trên kênh HBO?</t>
     <phoneticPr fontId="5"/>
   </si>
   <si>
@@ -5570,7 +5566,139 @@
     <phoneticPr fontId="5"/>
   </si>
   <si>
-    <t>Arrival 2016</t>
+    <t>Arrival</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>2024.12.08</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>7.2/10</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <r>
+      <t>Phim mãng xà ăn thịt người, trước thường được chiếu trên kênh HBO?
+Quả</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>ng cáo nhi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>ề</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve">u và gây </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>ấ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>n t</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>ư</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>ợ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t>ng</t>
+    </r>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Steve Jobs</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Start reading around 2024.10 …
+</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>In progress</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Focus on your goals, everything is important but some are more important. </t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>The richest man in Babylon</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>The personal MBA</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Factfulness: Ten Reasons We're Wrong About The World - And Why Things Are Better Than You Think</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Shinsekai yori</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>Hunter x Hunter</t>
     <phoneticPr fontId="5"/>
   </si>
 </sst>
@@ -5578,7 +5706,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="33" x14ac:knownFonts="1">
+  <fonts count="36" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5817,6 +5945,27 @@
       <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="游ゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="163"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="4">
@@ -6191,8 +6340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D1037"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD14"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6205,22 +6354,27 @@
   <sheetData>
     <row r="1" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="49" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="2" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
-        <v>1290</v>
+      <c r="B2" s="48" t="s">
+        <v>1223</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="48" t="s">
+        <v>1283</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="48" t="s">
-        <v>1224</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="48" t="s">
-        <v>1284</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6228,25 +6382,25 @@
     </row>
     <row r="8" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="43" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="52" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="48" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6254,27 +6408,27 @@
     </row>
     <row r="13" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="48" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="14" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="15" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="16" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="10" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="18" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6285,7 +6439,7 @@
     </row>
     <row r="20" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="49" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="21" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6350,7 +6504,7 @@
     </row>
     <row r="33" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="34" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -6375,10 +6529,10 @@
     </row>
     <row r="38" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="6" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="39" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -6407,7 +6561,7 @@
     </row>
     <row r="45" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="37" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="46" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -6436,7 +6590,7 @@
     </row>
     <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="43" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -6522,7 +6676,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B62" s="1" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -6641,7 +6795,7 @@
     <row r="84" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="85" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B85" s="3" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="86" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -6656,7 +6810,7 @@
     </row>
     <row r="88" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="89" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6709,20 +6863,20 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="101" spans="2:3" ht="55.5" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:3" ht="42" x14ac:dyDescent="0.25">
       <c r="B101" s="36" t="s">
         <v>1053</v>
       </c>
       <c r="C101" s="50" t="s">
-        <v>1228</v>
-      </c>
-    </row>
-    <row r="102" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B102" s="6" t="s">
+        <v>1167</v>
+      </c>
+      <c r="C102" s="5" t="s">
         <v>1168</v>
-      </c>
-      <c r="C102" s="5" t="s">
-        <v>1169</v>
       </c>
     </row>
     <row r="103" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -6735,20 +6889,20 @@
         <v>1020</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="105" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B105" s="6" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="106" spans="2:3" ht="39" x14ac:dyDescent="0.25">
       <c r="B106" s="53" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="C106" s="44" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="107" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -6758,28 +6912,28 @@
     </row>
     <row r="108" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B108" s="1" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="C108" s="54" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="109" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B109" s="1" t="s">
+        <v>1275</v>
+      </c>
+      <c r="C109" s="1" t="s">
         <v>1276</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>1277</v>
       </c>
     </row>
     <row r="110" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B110" s="55" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="111" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B111" s="21" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="112" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7725,8 +7879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G1008"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A322" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B153" sqref="B153"/>
+    <sheetView topLeftCell="A280" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A130" sqref="A130:XFD130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7882,7 +8036,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="C11" s="4"/>
       <c r="F11" s="1" t="s">
@@ -7924,7 +8078,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="C14" s="4"/>
       <c r="F14" s="1" t="s">
@@ -7936,7 +8090,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="C15" s="4"/>
       <c r="F15" s="1" t="s">
@@ -7963,7 +8117,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="C17" s="4"/>
       <c r="F17" s="1" t="s">
@@ -8111,11 +8265,11 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="C29" s="4"/>
       <c r="E29" s="16" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>54</v>
@@ -8129,7 +8283,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="C30" s="4">
         <v>2008</v>
@@ -8272,7 +8426,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="18">
@@ -8840,7 +8994,7 @@
         <v>42838</v>
       </c>
       <c r="E72" s="16" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>54</v>
@@ -8931,7 +9085,7 @@
     </row>
     <row r="77" spans="1:7" s="32" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="32" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="C77" s="45">
         <v>2009</v>
@@ -8939,7 +9093,7 @@
       <c r="D77" s="33"/>
       <c r="E77" s="46"/>
       <c r="G77" s="32" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -9468,7 +9622,7 @@
         <v>101</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="C103" s="4" t="s">
         <v>210</v>
@@ -9480,7 +9634,7 @@
         <v>54</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -9528,7 +9682,7 @@
         <v>104</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="C106" s="4">
         <v>2006</v>
@@ -9896,7 +10050,7 @@
         <v>123</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="C125" s="4" t="s">
         <v>1091</v>
@@ -9983,7 +10137,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" ht="33.75" x14ac:dyDescent="0.4">
       <c r="A130" s="1">
         <f t="shared" si="2"/>
         <v>128</v>
@@ -9997,8 +10151,8 @@
       <c r="F130" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G130" s="1" t="s">
-        <v>1132</v>
+      <c r="G130" s="12" t="s">
+        <v>1292</v>
       </c>
     </row>
     <row r="131" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -10038,7 +10192,7 @@
         <v>131</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="C133" s="4"/>
       <c r="F133" s="1" t="s">
@@ -10300,7 +10454,7 @@
         <v>150</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="C152" s="4"/>
       <c r="F152" s="1" t="s">
@@ -10313,7 +10467,7 @@
         <v>151</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="C153" s="4"/>
       <c r="F153" s="1" t="s">
@@ -10333,7 +10487,7 @@
         <v>248</v>
       </c>
       <c r="G154" s="12" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="155" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -10342,7 +10496,7 @@
         <v>153</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="C155" s="4"/>
       <c r="F155" s="1" t="s">
@@ -10394,7 +10548,7 @@
         <v>248</v>
       </c>
       <c r="G158" s="1" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="159" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -10801,7 +10955,7 @@
         <v>307</v>
       </c>
       <c r="C189" s="4" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="D189" s="18">
         <v>42797</v>
@@ -10991,7 +11145,7 @@
         <v>331</v>
       </c>
       <c r="C203" s="4" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="D203" s="18">
         <v>42925</v>
@@ -11543,7 +11697,7 @@
         <v>238</v>
       </c>
       <c r="B240" s="23" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="C240" s="22">
         <v>1997</v>
@@ -11630,14 +11784,14 @@
         <v>243</v>
       </c>
       <c r="B245" s="29" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="C245" s="4"/>
       <c r="D245" s="28" t="s">
         <v>1119</v>
       </c>
       <c r="G245" s="12" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="246" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -11676,7 +11830,7 @@
       </c>
       <c r="C248" s="4"/>
       <c r="G248" s="1" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="249" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -11994,7 +12148,7 @@
         <v>271</v>
       </c>
       <c r="B273" s="23" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="C273" s="22"/>
       <c r="D273" s="19"/>
@@ -12230,17 +12384,17 @@
     <row r="291" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A291" s="1"/>
       <c r="B291" s="8" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="C291" s="4"/>
       <c r="D291" s="28" t="s">
+        <v>1188</v>
+      </c>
+      <c r="E291" s="16" t="s">
         <v>1189</v>
       </c>
-      <c r="E291" s="16" t="s">
-        <v>1190</v>
-      </c>
       <c r="G291" s="1" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="292" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -12249,7 +12403,7 @@
         <v>289</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="C292" s="4">
         <v>2021</v>
@@ -12283,7 +12437,7 @@
         <v>291</v>
       </c>
       <c r="B294" s="29" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="C294" s="22"/>
       <c r="D294" s="19"/>
@@ -12294,7 +12448,7 @@
         <v>292</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="C295" s="4">
         <v>2022</v>
@@ -12413,7 +12567,7 @@
         <v>298</v>
       </c>
       <c r="B302" s="1" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="C302" s="4">
         <v>2022</v>
@@ -12442,7 +12596,7 @@
         <v>300</v>
       </c>
       <c r="B304" s="1" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="C304" s="4">
         <v>2017</v>
@@ -12454,7 +12608,7 @@
         <v>6.5</v>
       </c>
       <c r="G304" s="1" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="305" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -12462,7 +12616,7 @@
         <v>301</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="C305" s="4">
         <v>2022</v>
@@ -12502,7 +12656,7 @@
         <v>303</v>
       </c>
       <c r="B307" s="1" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="C307" s="4">
         <v>2001</v>
@@ -12522,7 +12676,7 @@
         <v>304</v>
       </c>
       <c r="B308" s="1" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="C308" s="4">
         <v>2022</v>
@@ -12539,7 +12693,7 @@
         <v>305</v>
       </c>
       <c r="B309" s="29" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="C309" s="4">
         <v>2023</v>
@@ -12583,7 +12737,7 @@
         <v>308</v>
       </c>
       <c r="B312" s="23" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="C312" s="27"/>
       <c r="D312" s="20" t="s">
@@ -12744,7 +12898,7 @@
         <v>1065</v>
       </c>
       <c r="G321" s="12" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="322" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -12752,16 +12906,16 @@
         <v>318</v>
       </c>
       <c r="B322" s="23" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="C322" s="4">
         <v>1988</v>
       </c>
       <c r="D322" s="28" t="s">
+        <v>1179</v>
+      </c>
+      <c r="G322" s="6" t="s">
         <v>1180</v>
-      </c>
-      <c r="G322" s="6" t="s">
-        <v>1181</v>
       </c>
     </row>
     <row r="323" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -12769,29 +12923,29 @@
         <v>319</v>
       </c>
       <c r="B323" s="23" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="C323" s="4"/>
       <c r="D323" s="28" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="E323" s="17" t="s">
         <v>1112</v>
       </c>
       <c r="G323" s="1" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="324" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A324" s="1"/>
       <c r="B324" s="23" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="C324" s="4"/>
       <c r="D324" s="28"/>
       <c r="E324" s="17"/>
       <c r="G324" s="1" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="325" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -12799,14 +12953,14 @@
         <v>320</v>
       </c>
       <c r="B325" s="24" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="C325" s="4"/>
       <c r="E325" s="47" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="G325" s="1" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="326" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -12814,17 +12968,17 @@
         <v>321</v>
       </c>
       <c r="B326" s="24" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="C326" s="4"/>
       <c r="D326" s="28" t="s">
+        <v>1196</v>
+      </c>
+      <c r="E326" s="47" t="s">
         <v>1197</v>
       </c>
-      <c r="E326" s="47" t="s">
-        <v>1198</v>
-      </c>
       <c r="G326" s="1" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="327" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -12832,17 +12986,17 @@
         <v>322</v>
       </c>
       <c r="B327" s="24" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="C327" s="4"/>
       <c r="D327" s="28" t="s">
+        <v>1214</v>
+      </c>
+      <c r="E327" s="47" t="s">
+        <v>1242</v>
+      </c>
+      <c r="G327" s="1" t="s">
         <v>1215</v>
-      </c>
-      <c r="E327" s="47" t="s">
-        <v>1243</v>
-      </c>
-      <c r="G327" s="1" t="s">
-        <v>1216</v>
       </c>
     </row>
     <row r="328" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -12850,16 +13004,16 @@
         <v>323</v>
       </c>
       <c r="B328" s="24" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D328" s="28" t="s">
+        <v>1213</v>
+      </c>
+      <c r="E328" s="47" t="s">
         <v>1219</v>
       </c>
-      <c r="D328" s="28" t="s">
-        <v>1214</v>
-      </c>
-      <c r="E328" s="47" t="s">
-        <v>1220</v>
-      </c>
       <c r="G328" s="1" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="329" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -12867,13 +13021,13 @@
         <v>324</v>
       </c>
       <c r="B329" s="51" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="C329" s="4">
         <v>2015</v>
       </c>
       <c r="D329" s="28" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="E329" s="47" t="s">
         <v>1065</v>
@@ -12884,19 +13038,19 @@
         <v>325</v>
       </c>
       <c r="B330" s="24" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="C330" s="4">
         <v>2000</v>
       </c>
       <c r="D330" s="28" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="E330" s="47" t="s">
         <v>1112</v>
       </c>
       <c r="G330" s="1" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="331" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -12904,19 +13058,19 @@
         <v>326</v>
       </c>
       <c r="B331" s="24" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="C331" s="4">
         <v>2023</v>
       </c>
       <c r="D331" s="28" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="E331" s="47" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="G331" s="21" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="332" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -12924,13 +13078,13 @@
         <v>327</v>
       </c>
       <c r="B332" s="24" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="C332" s="4">
         <v>1995</v>
       </c>
       <c r="D332" s="28" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="333" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -12938,16 +13092,16 @@
         <v>328</v>
       </c>
       <c r="B333" s="24" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="C333" s="4">
         <v>2014</v>
       </c>
       <c r="D333" s="28" t="s">
+        <v>1271</v>
+      </c>
+      <c r="E333" s="47" t="s">
         <v>1272</v>
-      </c>
-      <c r="E333" s="47" t="s">
-        <v>1273</v>
       </c>
     </row>
     <row r="334" spans="1:7" s="32" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -12955,20 +13109,34 @@
         <v>329</v>
       </c>
       <c r="B334" s="32" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="C334" s="45">
         <v>2024</v>
       </c>
       <c r="D334" s="33" t="s">
+        <v>1285</v>
+      </c>
+      <c r="E334" s="46" t="s">
         <v>1286</v>
       </c>
-      <c r="E334" s="46" t="s">
-        <v>1287</v>
-      </c>
     </row>
     <row r="335" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C335" s="4"/>
+      <c r="A335" s="1">
+        <v>330</v>
+      </c>
+      <c r="B335" s="24" t="s">
+        <v>1289</v>
+      </c>
+      <c r="C335" s="4">
+        <v>2016</v>
+      </c>
+      <c r="D335" s="28" t="s">
+        <v>1290</v>
+      </c>
+      <c r="E335" s="16" t="s">
+        <v>1291</v>
+      </c>
     </row>
     <row r="336" spans="1:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C336" s="4"/>
@@ -14998,10 +15166,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H1008"/>
+  <dimension ref="A1:H1009"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -15020,10 +15188,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1051</v>
@@ -15053,7 +15221,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="42" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="C3" s="38" t="s">
         <v>587</v>
@@ -15179,7 +15347,7 @@
         <v>598</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -15231,7 +15399,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>1038</v>
@@ -15514,13 +15682,13 @@
         <v>13</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>511</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
@@ -15599,7 +15767,7 @@
     </row>
     <row r="48" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="13" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="49" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -15609,127 +15777,152 @@
     </row>
     <row r="50" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="31" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="51" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="31" t="s">
+        <v>1162</v>
+      </c>
+      <c r="E51" s="1" t="s">
         <v>1163</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>1164</v>
       </c>
     </row>
     <row r="52" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="31" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="E52" s="1" t="s">
+        <v>1246</v>
+      </c>
+      <c r="F52" s="1" t="s">
         <v>1247</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>1248</v>
       </c>
     </row>
     <row r="53" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="31" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="54" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="31" t="s">
+        <v>1248</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>1249</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>1250</v>
-      </c>
       <c r="E54" s="1"/>
+      <c r="F54" s="1" t="s">
+        <v>1296</v>
+      </c>
     </row>
     <row r="55" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="31" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>1253</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>1254</v>
       </c>
       <c r="E55" s="1"/>
     </row>
     <row r="56" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="31" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="C56" s="1"/>
       <c r="E56" s="1" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="57" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="31" t="s">
+        <v>1297</v>
+      </c>
+      <c r="C57" s="1"/>
       <c r="E57" s="1"/>
     </row>
-    <row r="58" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="31"/>
-      <c r="C58" s="1"/>
-      <c r="E58" s="1"/>
-    </row>
-    <row r="59" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="8" t="s">
-        <v>1175</v>
-      </c>
-    </row>
+    <row r="58" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B58" s="31" t="s">
+        <v>1293</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>1295</v>
+      </c>
+      <c r="F58" s="12" t="s">
+        <v>1294</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="31"/>
+      <c r="C59" s="1"/>
+      <c r="E59" s="1"/>
+    </row>
+    <row r="60" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="61" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="1" t="s">
+      <c r="B61" s="8" t="s">
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="1" t="s">
         <v>989</v>
       </c>
     </row>
-    <row r="62" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="63" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="64" spans="2:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="65" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="66" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="67" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="43" t="s">
-        <v>1176</v>
-      </c>
-    </row>
-    <row r="69" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="43" t="s">
+        <v>1175</v>
+      </c>
+    </row>
     <row r="70" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="71" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="72" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="73" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="8" t="s">
+    <row r="74" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B75" s="8" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B76" s="31" t="s">
         <v>1257</v>
       </c>
-    </row>
-    <row r="75" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="31" t="s">
-        <v>1258</v>
-      </c>
-      <c r="C75" s="1" t="s">
+      <c r="C76" s="1" t="s">
         <v>1030</v>
-      </c>
-    </row>
-    <row r="76" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="1" t="s">
-        <v>1259</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>1260</v>
       </c>
     </row>
     <row r="77" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="1" t="s">
-        <v>1262</v>
-      </c>
-    </row>
-    <row r="78" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>1258</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B78" s="1" t="s">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B79" s="1" t="s">
+        <v>1298</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B80" s="12" t="s">
+        <v>1299</v>
+      </c>
+    </row>
     <row r="81" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="82" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="83" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -16658,6 +16851,7 @@
     <row r="1006" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1007" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1008" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1009" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="5"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -16681,12 +16875,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
     </row>
   </sheetData>
@@ -16770,7 +16964,7 @@
         <v>496</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -18312,37 +18506,37 @@
     <row r="53" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="54" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="8" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="8" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>